<commit_message>
Date:2016-04-09 Description：git持续学习ignore,add -u git config alias
</commit_message>
<xml_diff>
--- a/NoteBook.xlsx
+++ b/NoteBook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="26860" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="目录" sheetId="1" r:id="rId1"/>
@@ -16,8 +16,8 @@
   </sheets>
   <definedNames>
     <definedName name="Git_管理本地仓库">Git的使用!$C$17</definedName>
-    <definedName name="Git_配置">Git的使用!$C$247</definedName>
-    <definedName name="Git_与远程主机的交互">Git的使用!$C$120</definedName>
+    <definedName name="Git_配置">Git的使用!$C$255</definedName>
+    <definedName name="Git_与远程主机的交互">Git的使用!$C$128</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="312">
   <si>
     <t>#else</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -592,10 +592,6 @@
   </si>
   <si>
     <t>git add .</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>将所有新增/修改的文件提交到暂存区</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1090,35 +1086,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>.DS_Store // 忽略所有的.DS_Store文件</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>*.a       // 忽略所有的以a为扩展名的文件</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Temp/    // 忽略根目录下的Temp文件夹下的所有文件</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Temp     // 忽略根目录下的Temp文件</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Temp/a.h // 忽略根目录下的Temp文件夹下的a.h</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>!lib.a    // 不忽略lib.a(在上一种情况下,可以设置忽略某一种类型,但特例除外</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>备注</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>如果在创建并设置.gitignore之前,就已经追踪了某写文件,那么这些文件不受gitignore配置的影响</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1485,6 +1453,122 @@
       </rPr>
       <t>)</t>
     </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>config文件的配置</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用途</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git config commit.template &lt;文件名&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git config commit.template /commit_template/default.txt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>将commit_template目录下的 default.txt 文件作为commit 模板</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果想删除该项配置则利用 --unset</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git config --unset commit.template</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>~\$*.xlsx   // 忽略excel的编辑临时文件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Temp/a.h   // 忽略根目录下的Temp文件夹下的a.h</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Temp       // 忽略根目录下的Temp文件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Temp/      // 忽略根目录下的Temp文件夹下的所有文件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>!lib.a      // 不忽略lib.a(在上一种情况下,可以设置忽略某一种类型,但特例除外</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>.DS_Store   // 忽略所有的.DS_Store文件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>*.a         // 忽略所有的以a为扩展名的文件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果在创建并设置.gitignore之前,就已经追踪了某些文件,那么这些文件不受gitignore配置的影响</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>对git的环境进行配置,如用户名,commit信息模板,命令别名等</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">git config alias.&lt;alias name&gt; &lt;commands&gt; </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git config alias.st status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>将"st" 作为" status"的别名,则 git st ==&gt;git status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>取消这项配置:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git config --unset alias.st</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git add -u</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>将workspace中有更新的且被追踪了的文件提交到暂存区</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>另外</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>在改了很多文件,又新增了不少文件的情况,我可能只关心修改的,而先不管新增的,那么这个命令就很有用</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>将递归当前目录下所有新增/修改的文件提交到暂存区,如果把"."换成某一个目录,则只会递归该目录</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git add -i</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>交互式的添加</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1858,13 +1942,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>219</xdr:row>
+      <xdr:row>227</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>243</xdr:row>
+      <xdr:row>251</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1896,7 +1980,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="7791450" cy="5133975"/>
@@ -1929,13 +2013,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2376,7 +2460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" topLeftCell="A5" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0"/>
   <cols>
@@ -2411,17 +2495,17 @@
     </row>
     <row r="12" spans="2:4">
       <c r="C12" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="D13" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="D14" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -2437,7 +2521,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -2460,7 +2544,7 @@
     </row>
     <row r="23" spans="2:4">
       <c r="D23" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2495,7 +2579,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2755,10 +2839,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N266"/>
+  <dimension ref="A1:N295"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="C266" sqref="C266"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0"/>
@@ -2772,24 +2856,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" s="25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3">
       <c r="B3" s="25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -2799,14 +2883,14 @@
     </row>
     <row r="6" spans="1:3">
       <c r="B6" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" s="3"/>
       <c r="C7" s="5" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2827,20 +2911,20 @@
     </row>
     <row r="12" spans="1:3">
       <c r="B12" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3">
       <c r="B13" s="26" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3">
       <c r="B14" s="24"/>
       <c r="C14" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="2:5">
@@ -2848,12 +2932,12 @@
         <v>1</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="C18" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>128</v>
@@ -2864,7 +2948,7 @@
         <v>129</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20" spans="2:5">
@@ -2899,761 +2983,681 @@
       </c>
     </row>
     <row r="25" spans="2:5">
+      <c r="D25" s="5" t="s">
+        <v>307</v>
+      </c>
       <c r="E25" s="6" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="26" spans="2:5">
       <c r="E26" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="E28" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="E29" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="E30" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="E32" s="5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5">
+      <c r="E33" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5">
+      <c r="D36" s="5" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="D28" s="5" t="s">
+      <c r="E36" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E28" s="6" t="s">
+    </row>
+    <row r="37" spans="3:5">
+      <c r="E37" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="2:5">
-      <c r="E29" s="7" t="s">
+    <row r="39" spans="3:5">
+      <c r="C39" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="2:5">
-      <c r="C31" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D31" s="5" t="s">
+    <row r="40" spans="3:5">
+      <c r="D40" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="2:5">
-      <c r="D32" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="4:5">
-      <c r="D33" s="5" t="s">
+    <row r="41" spans="3:5">
+      <c r="D41" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E41" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5">
+      <c r="E42" s="5" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="34" spans="4:5">
-      <c r="E34" s="5" t="s">
+    <row r="44" spans="3:5">
+      <c r="D44" s="5" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="36" spans="4:5">
-      <c r="D36" s="5" t="s">
+      <c r="E44" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5">
+      <c r="E45" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="37" spans="4:5">
-      <c r="E37" s="5" t="s">
+    </row>
+    <row r="46" spans="3:5">
+      <c r="E46" s="5" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="38" spans="4:5">
-      <c r="E38" s="5" t="s">
+    <row r="47" spans="3:5">
+      <c r="E47" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="39" spans="4:5">
-      <c r="E39" s="5" t="s">
+    <row r="48" spans="3:5">
+      <c r="E48" s="5" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="40" spans="4:5">
-      <c r="E40" s="5" t="s">
+    <row r="49" spans="4:13">
+      <c r="E49" s="5" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="41" spans="4:5">
-      <c r="E41" s="5" t="s">
+    <row r="50" spans="4:13">
+      <c r="E50" s="5" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="42" spans="4:5">
-      <c r="E42" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="44" spans="4:5">
-      <c r="D44" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="45" spans="4:5">
-      <c r="E45" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="46" spans="4:5">
-      <c r="E46" s="6" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="47" spans="4:5">
-      <c r="E47" s="5" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="48" spans="4:5">
-      <c r="E48" s="5" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="52" spans="4:13">
       <c r="D52" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="53" spans="4:13">
+      <c r="E53" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="54" spans="4:13">
+      <c r="E54" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="55" spans="4:13">
+      <c r="E55" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="56" spans="4:13">
+      <c r="E56" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="60" spans="4:13">
+      <c r="D60" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="M60" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="M52" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="80" spans="3:4">
-      <c r="C80" s="24" t="s">
-        <v>217</v>
-      </c>
-      <c r="D80" s="5" t="s">
+    </row>
+    <row r="88" spans="3:6">
+      <c r="C88" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6">
+      <c r="D89" s="5" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="81" spans="4:6">
-      <c r="D81" s="5" t="s">
+      <c r="E89" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="E81" s="5" t="s">
+    </row>
+    <row r="90" spans="3:6">
+      <c r="D90" s="5" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="82" spans="4:6">
-      <c r="D82" s="5" t="s">
+      <c r="E90" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="E82" s="5" t="s">
+    </row>
+    <row r="91" spans="3:6">
+      <c r="E91" s="5">
+        <v>1</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="92" spans="3:6">
+      <c r="F92" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="94" spans="3:6">
+      <c r="E94" s="5">
+        <v>2</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="95" spans="3:6">
+      <c r="F95" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="97" spans="4:6">
+      <c r="E97" s="5">
+        <v>3</v>
+      </c>
+      <c r="F97" s="5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="83" spans="4:6">
-      <c r="E83" s="5">
+    <row r="98" spans="4:6">
+      <c r="F98" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6">
+      <c r="D100" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6">
+      <c r="E101" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="102" spans="4:6">
+      <c r="E102" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="103" spans="4:6">
+      <c r="E103" s="5">
         <v>1</v>
       </c>
-      <c r="F83" s="5" t="s">
+      <c r="F103" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="104" spans="4:6">
+      <c r="F104" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="105" spans="4:6">
+      <c r="E105" s="5">
+        <v>2</v>
+      </c>
+      <c r="F105" s="5" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="84" spans="4:6">
-      <c r="F84" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="86" spans="4:6">
-      <c r="E86" s="5">
-        <v>2</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="87" spans="4:6">
-      <c r="F87" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="89" spans="4:6">
-      <c r="E89" s="5">
+    <row r="106" spans="4:6">
+      <c r="F106" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="107" spans="4:6">
+      <c r="F107" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="4:6">
+      <c r="F108" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="109" spans="4:6">
+      <c r="F109" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="110" spans="4:6">
+      <c r="F110" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="111" spans="4:6">
+      <c r="E111" s="5">
         <v>3</v>
       </c>
-      <c r="F89" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="90" spans="4:6">
-      <c r="F90" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="92" spans="4:6">
-      <c r="D92" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="93" spans="4:6">
-      <c r="E93" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="94" spans="4:6">
-      <c r="E94" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="95" spans="4:6">
-      <c r="E95" s="5">
-        <v>1</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="96" spans="4:6">
-      <c r="F96" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="97" spans="5:6">
-      <c r="E97" s="5">
-        <v>2</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="98" spans="5:6">
-      <c r="F98" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="99" spans="5:6">
-      <c r="F99" s="5" t="s">
+      <c r="F111" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="100" spans="5:6">
-      <c r="F100" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="101" spans="5:6">
-      <c r="F101" s="5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="102" spans="5:6">
-      <c r="F102" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="103" spans="5:6">
-      <c r="E103" s="5">
-        <v>3</v>
-      </c>
-      <c r="F103" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="104" spans="5:6">
-      <c r="F104" s="5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="105" spans="5:6">
-      <c r="F105" s="5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="106" spans="5:6">
-      <c r="F106" s="5" t="s">
+    <row r="112" spans="4:6">
+      <c r="F112" s="5" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="107" spans="5:6">
-      <c r="E107" s="5">
-        <v>4</v>
-      </c>
-      <c r="F107" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="108" spans="5:6">
-      <c r="F108" s="5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="109" spans="5:6">
-      <c r="F109" s="5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="110" spans="5:6">
-      <c r="F110" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="111" spans="5:6">
-      <c r="E111" s="5">
-        <v>5</v>
-      </c>
-      <c r="F111" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="112" spans="5:6">
-      <c r="F112" s="5" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="113" spans="2:6">
       <c r="F113" s="5" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="114" spans="2:6">
       <c r="F114" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6">
+      <c r="E115" s="5">
+        <v>4</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6">
+      <c r="F116" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6">
+      <c r="F117" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6">
+      <c r="F118" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6">
+      <c r="E119" s="5">
+        <v>5</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6">
+      <c r="F120" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6">
+      <c r="F121" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6">
+      <c r="F122" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6">
+      <c r="F123" s="5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="115" spans="2:6">
-      <c r="F115" s="5" t="s">
+    <row r="124" spans="2:6">
+      <c r="E124" s="5">
+        <v>6</v>
+      </c>
+      <c r="F124" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="116" spans="2:6">
-      <c r="E116" s="5">
-        <v>6</v>
-      </c>
-      <c r="F116" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6">
-      <c r="B120" s="22">
+    <row r="128" spans="2:6">
+      <c r="B128" s="22">
         <v>2</v>
       </c>
-      <c r="C120" s="25" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6">
-      <c r="C121" s="24" t="s">
+      <c r="C128" s="25" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="129" spans="3:11">
+      <c r="C129" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="131" spans="3:11">
+      <c r="D131" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="132" spans="3:11">
+      <c r="D132" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="133" spans="3:11">
+      <c r="D133" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="134" spans="3:11">
+      <c r="E134" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="136" spans="3:11">
+      <c r="E136" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="137" spans="3:11">
+      <c r="E137" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="138" spans="3:11">
+      <c r="E138" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="140" spans="3:11">
+      <c r="C140" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="D121" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6">
-      <c r="D123" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E123" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6">
-      <c r="D124" s="5" t="s">
+      <c r="D140" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="142" spans="3:11">
+      <c r="D142" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E142" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="143" spans="3:11">
+      <c r="D143" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E143" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="144" spans="3:11">
+      <c r="E144" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F144" s="9"/>
+      <c r="G144" s="9"/>
+      <c r="H144" s="9"/>
+      <c r="I144" s="9"/>
+      <c r="J144" s="9"/>
+      <c r="K144" s="10"/>
+    </row>
+    <row r="145" spans="3:12">
+      <c r="E145" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F145" s="12"/>
+      <c r="G145" s="12"/>
+      <c r="H145" s="12"/>
+      <c r="I145" s="12"/>
+      <c r="J145" s="12"/>
+      <c r="K145" s="13"/>
+    </row>
+    <row r="146" spans="3:12">
+      <c r="E146" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F146" s="12"/>
+      <c r="G146" s="12"/>
+      <c r="H146" s="12"/>
+      <c r="I146" s="12"/>
+      <c r="J146" s="12"/>
+      <c r="K146" s="13"/>
+    </row>
+    <row r="147" spans="3:12">
+      <c r="E147" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F147" s="15"/>
+      <c r="G147" s="15"/>
+      <c r="H147" s="15"/>
+      <c r="I147" s="15"/>
+      <c r="J147" s="15"/>
+      <c r="K147" s="16"/>
+    </row>
+    <row r="149" spans="3:12">
+      <c r="E149" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="150" spans="3:12">
+      <c r="E150" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F150" s="9"/>
+      <c r="G150" s="9"/>
+      <c r="H150" s="9"/>
+      <c r="I150" s="9"/>
+      <c r="J150" s="9"/>
+      <c r="K150" s="9"/>
+      <c r="L150" s="10"/>
+    </row>
+    <row r="151" spans="3:12">
+      <c r="E151" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F151" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="G151" s="12"/>
+      <c r="H151" s="12"/>
+      <c r="I151" s="12"/>
+      <c r="J151" s="12"/>
+      <c r="K151" s="12"/>
+      <c r="L151" s="13"/>
+    </row>
+    <row r="152" spans="3:12">
+      <c r="E152" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F152" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G152" s="15"/>
+      <c r="H152" s="15"/>
+      <c r="I152" s="15"/>
+      <c r="J152" s="15"/>
+      <c r="K152" s="15"/>
+      <c r="L152" s="16"/>
+    </row>
+    <row r="154" spans="3:12">
+      <c r="C154" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D154" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="156" spans="3:12">
+      <c r="D156" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E156" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="157" spans="3:12">
+      <c r="D157" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E124" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="125" spans="2:6">
-      <c r="D125" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E125" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="126" spans="2:6">
-      <c r="E126" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="128" spans="2:6">
-      <c r="E128" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="129" spans="3:12">
-      <c r="E129" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="130" spans="3:12">
-      <c r="E130" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="132" spans="3:12">
-      <c r="C132" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="D132" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="134" spans="3:12">
-      <c r="D134" s="5" t="s">
+      <c r="E157" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="158" spans="3:12">
+      <c r="E158" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="159" spans="3:12">
+      <c r="D159" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E159" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="160" spans="3:12">
+      <c r="E160" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="161" spans="3:5">
+      <c r="E161" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="162" spans="3:5">
+      <c r="E162" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="163" spans="3:5">
+      <c r="E163" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="164" spans="3:5">
+      <c r="E164" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="165" spans="3:5">
+      <c r="E165" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="167" spans="3:5">
+      <c r="C167" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D167" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="169" spans="3:5">
+      <c r="D169" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E134" s="5" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="135" spans="3:12">
-      <c r="D135" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E135" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="136" spans="3:12">
-      <c r="E136" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F136" s="9"/>
-      <c r="G136" s="9"/>
-      <c r="H136" s="9"/>
-      <c r="I136" s="9"/>
-      <c r="J136" s="9"/>
-      <c r="K136" s="10"/>
-    </row>
-    <row r="137" spans="3:12">
-      <c r="E137" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F137" s="12"/>
-      <c r="G137" s="12"/>
-      <c r="H137" s="12"/>
-      <c r="I137" s="12"/>
-      <c r="J137" s="12"/>
-      <c r="K137" s="13"/>
-    </row>
-    <row r="138" spans="3:12">
-      <c r="E138" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F138" s="12"/>
-      <c r="G138" s="12"/>
-      <c r="H138" s="12"/>
-      <c r="I138" s="12"/>
-      <c r="J138" s="12"/>
-      <c r="K138" s="13"/>
-    </row>
-    <row r="139" spans="3:12">
-      <c r="E139" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F139" s="15"/>
-      <c r="G139" s="15"/>
-      <c r="H139" s="15"/>
-      <c r="I139" s="15"/>
-      <c r="J139" s="15"/>
-      <c r="K139" s="16"/>
-    </row>
-    <row r="141" spans="3:12">
-      <c r="E141" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="142" spans="3:12">
-      <c r="E142" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F142" s="9"/>
-      <c r="G142" s="9"/>
-      <c r="H142" s="9"/>
-      <c r="I142" s="9"/>
-      <c r="J142" s="9"/>
-      <c r="K142" s="9"/>
-      <c r="L142" s="10"/>
-    </row>
-    <row r="143" spans="3:12">
-      <c r="E143" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F143" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="G143" s="12"/>
-      <c r="H143" s="12"/>
-      <c r="I143" s="12"/>
-      <c r="J143" s="12"/>
-      <c r="K143" s="12"/>
-      <c r="L143" s="13"/>
-    </row>
-    <row r="144" spans="3:12">
-      <c r="E144" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F144" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G144" s="15"/>
-      <c r="H144" s="15"/>
-      <c r="I144" s="15"/>
-      <c r="J144" s="15"/>
-      <c r="K144" s="15"/>
-      <c r="L144" s="16"/>
-    </row>
-    <row r="146" spans="3:5">
-      <c r="C146" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="D146" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="148" spans="3:5">
-      <c r="D148" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E148" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="149" spans="3:5">
-      <c r="D149" s="5" t="s">
+      <c r="E169" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="170" spans="3:5">
+      <c r="D170" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E149" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="150" spans="3:5">
-      <c r="E150" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="151" spans="3:5">
-      <c r="D151" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E151" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="152" spans="3:5">
-      <c r="E152" s="5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="153" spans="3:5">
-      <c r="E153" s="5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="154" spans="3:5">
-      <c r="E154" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="155" spans="3:5">
-      <c r="E155" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="156" spans="3:5">
-      <c r="E156" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="157" spans="3:5">
-      <c r="E157" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="159" spans="3:5">
-      <c r="C159" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="D159" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="161" spans="4:14">
-      <c r="D161" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E161" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="162" spans="4:14">
-      <c r="D162" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E162" s="5" t="s">
+      <c r="E170" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="163" spans="4:14">
-      <c r="D163" s="5" t="s">
+    <row r="171" spans="3:5">
+      <c r="D171" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E163" s="5" t="s">
+      <c r="E171" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="164" spans="4:14">
-      <c r="E164" s="5" t="s">
+    <row r="172" spans="3:5">
+      <c r="E172" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="165" spans="4:14">
-      <c r="E165" s="5" t="s">
+    <row r="173" spans="3:5">
+      <c r="E173" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="168" spans="4:14">
-      <c r="D168" s="5" t="s">
+    <row r="176" spans="3:5">
+      <c r="D176" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E168" s="5" t="s">
+      <c r="E176" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="169" spans="4:14">
-      <c r="E169" s="5" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="170" spans="4:14">
-      <c r="E170" s="8" t="s">
+    <row r="177" spans="5:14">
+      <c r="E177" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="178" spans="5:14">
+      <c r="E178" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F170" s="9"/>
-      <c r="G170" s="9"/>
-      <c r="H170" s="9"/>
-      <c r="I170" s="9"/>
-      <c r="J170" s="9"/>
-      <c r="K170" s="9"/>
-      <c r="L170" s="9"/>
-      <c r="M170" s="9"/>
-      <c r="N170" s="10"/>
-    </row>
-    <row r="171" spans="4:14">
-      <c r="E171" s="11" t="s">
+      <c r="F178" s="9"/>
+      <c r="G178" s="9"/>
+      <c r="H178" s="9"/>
+      <c r="I178" s="9"/>
+      <c r="J178" s="9"/>
+      <c r="K178" s="9"/>
+      <c r="L178" s="9"/>
+      <c r="M178" s="9"/>
+      <c r="N178" s="10"/>
+    </row>
+    <row r="179" spans="5:14">
+      <c r="E179" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F171" s="12"/>
-      <c r="G171" s="12"/>
-      <c r="H171" s="12"/>
-      <c r="I171" s="12"/>
-      <c r="J171" s="12"/>
-      <c r="K171" s="12"/>
-      <c r="L171" s="12"/>
-      <c r="M171" s="12"/>
-      <c r="N171" s="13"/>
-    </row>
-    <row r="172" spans="4:14">
-      <c r="E172" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F172" s="12"/>
-      <c r="G172" s="12"/>
-      <c r="H172" s="12"/>
-      <c r="I172" s="12"/>
-      <c r="J172" s="12"/>
-      <c r="K172" s="12"/>
-      <c r="L172" s="12"/>
-      <c r="M172" s="12"/>
-      <c r="N172" s="13"/>
-    </row>
-    <row r="173" spans="4:14">
-      <c r="E173" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F173" s="12"/>
-      <c r="G173" s="12"/>
-      <c r="H173" s="12"/>
-      <c r="I173" s="12"/>
-      <c r="J173" s="12"/>
-      <c r="K173" s="12"/>
-      <c r="L173" s="12"/>
-      <c r="M173" s="12"/>
-      <c r="N173" s="13"/>
-    </row>
-    <row r="174" spans="4:14">
-      <c r="E174" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F174" s="12"/>
-      <c r="G174" s="12"/>
-      <c r="H174" s="12"/>
-      <c r="I174" s="12"/>
-      <c r="J174" s="12"/>
-      <c r="K174" s="12"/>
-      <c r="L174" s="12"/>
-      <c r="M174" s="12"/>
-      <c r="N174" s="13"/>
-    </row>
-    <row r="175" spans="4:14">
-      <c r="E175" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F175" s="12"/>
-      <c r="G175" s="12"/>
-      <c r="H175" s="12"/>
-      <c r="I175" s="12"/>
-      <c r="J175" s="12"/>
-      <c r="K175" s="12"/>
-      <c r="L175" s="12"/>
-      <c r="M175" s="12"/>
-      <c r="N175" s="13"/>
-    </row>
-    <row r="176" spans="4:14">
-      <c r="E176" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="F176" s="12"/>
-      <c r="G176" s="12"/>
-      <c r="H176" s="12"/>
-      <c r="I176" s="12"/>
-      <c r="J176" s="12"/>
-      <c r="K176" s="12"/>
-      <c r="L176" s="12"/>
-      <c r="M176" s="12"/>
-      <c r="N176" s="13"/>
-    </row>
-    <row r="177" spans="5:14">
-      <c r="E177" s="11"/>
-      <c r="F177" s="12"/>
-      <c r="G177" s="12"/>
-      <c r="H177" s="12"/>
-      <c r="I177" s="12"/>
-      <c r="J177" s="12"/>
-      <c r="K177" s="12"/>
-      <c r="L177" s="12"/>
-      <c r="M177" s="12"/>
-      <c r="N177" s="13"/>
-    </row>
-    <row r="178" spans="5:14">
-      <c r="E178" s="11"/>
-      <c r="F178" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="G178" s="12"/>
-      <c r="H178" s="12"/>
-      <c r="I178" s="12"/>
-      <c r="J178" s="12"/>
-      <c r="K178" s="12"/>
-      <c r="L178" s="12"/>
-      <c r="M178" s="12"/>
-      <c r="N178" s="13"/>
-    </row>
-    <row r="179" spans="5:14">
-      <c r="E179" s="11"/>
       <c r="F179" s="12"/>
       <c r="G179" s="12"/>
       <c r="H179" s="12"/>
@@ -3666,7 +3670,7 @@
     </row>
     <row r="180" spans="5:14">
       <c r="E180" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F180" s="12"/>
       <c r="G180" s="12"/>
@@ -3680,7 +3684,7 @@
     </row>
     <row r="181" spans="5:14">
       <c r="E181" s="11" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="F181" s="12"/>
       <c r="G181" s="12"/>
@@ -3693,345 +3697,530 @@
       <c r="N181" s="13"/>
     </row>
     <row r="182" spans="5:14">
-      <c r="E182" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="F182" s="19"/>
-      <c r="G182" s="19"/>
-      <c r="H182" s="19"/>
-      <c r="I182" s="19"/>
-      <c r="J182" s="19"/>
-      <c r="K182" s="19"/>
-      <c r="L182" s="19"/>
+      <c r="E182" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F182" s="12"/>
+      <c r="G182" s="12"/>
+      <c r="H182" s="12"/>
+      <c r="I182" s="12"/>
+      <c r="J182" s="12"/>
+      <c r="K182" s="12"/>
+      <c r="L182" s="12"/>
       <c r="M182" s="12"/>
       <c r="N182" s="13"/>
     </row>
     <row r="183" spans="5:14">
-      <c r="E183" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="F183" s="19"/>
-      <c r="G183" s="19"/>
-      <c r="H183" s="19"/>
-      <c r="I183" s="19"/>
-      <c r="J183" s="19"/>
-      <c r="K183" s="19"/>
-      <c r="L183" s="19"/>
+      <c r="E183" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F183" s="12"/>
+      <c r="G183" s="12"/>
+      <c r="H183" s="12"/>
+      <c r="I183" s="12"/>
+      <c r="J183" s="12"/>
+      <c r="K183" s="12"/>
+      <c r="L183" s="12"/>
       <c r="M183" s="12"/>
       <c r="N183" s="13"/>
     </row>
     <row r="184" spans="5:14">
-      <c r="E184" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F184" s="19"/>
-      <c r="G184" s="19"/>
-      <c r="H184" s="19"/>
-      <c r="I184" s="19"/>
-      <c r="J184" s="19"/>
-      <c r="K184" s="19"/>
-      <c r="L184" s="19"/>
+      <c r="E184" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F184" s="12"/>
+      <c r="G184" s="12"/>
+      <c r="H184" s="12"/>
+      <c r="I184" s="12"/>
+      <c r="J184" s="12"/>
+      <c r="K184" s="12"/>
+      <c r="L184" s="12"/>
       <c r="M184" s="12"/>
       <c r="N184" s="13"/>
     </row>
     <row r="185" spans="5:14">
-      <c r="E185" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F185" s="19"/>
-      <c r="G185" s="19"/>
-      <c r="H185" s="19"/>
-      <c r="I185" s="19"/>
-      <c r="J185" s="19"/>
-      <c r="K185" s="19"/>
-      <c r="L185" s="19"/>
+      <c r="E185" s="11"/>
+      <c r="F185" s="12"/>
+      <c r="G185" s="12"/>
+      <c r="H185" s="12"/>
+      <c r="I185" s="12"/>
+      <c r="J185" s="12"/>
+      <c r="K185" s="12"/>
+      <c r="L185" s="12"/>
       <c r="M185" s="12"/>
       <c r="N185" s="13"/>
     </row>
     <row r="186" spans="5:14">
-      <c r="E186" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="F186" s="19"/>
-      <c r="G186" s="19"/>
-      <c r="H186" s="19"/>
-      <c r="I186" s="19"/>
-      <c r="J186" s="19"/>
-      <c r="K186" s="19"/>
-      <c r="L186" s="19"/>
+      <c r="E186" s="11"/>
+      <c r="F186" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G186" s="12"/>
+      <c r="H186" s="12"/>
+      <c r="I186" s="12"/>
+      <c r="J186" s="12"/>
+      <c r="K186" s="12"/>
+      <c r="L186" s="12"/>
       <c r="M186" s="12"/>
       <c r="N186" s="13"/>
     </row>
     <row r="187" spans="5:14">
-      <c r="E187" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F187" s="19"/>
-      <c r="G187" s="19"/>
-      <c r="H187" s="19"/>
-      <c r="I187" s="19"/>
-      <c r="J187" s="19"/>
-      <c r="K187" s="19"/>
-      <c r="L187" s="19"/>
+      <c r="E187" s="11"/>
+      <c r="F187" s="12"/>
+      <c r="G187" s="12"/>
+      <c r="H187" s="12"/>
+      <c r="I187" s="12"/>
+      <c r="J187" s="12"/>
+      <c r="K187" s="12"/>
+      <c r="L187" s="12"/>
       <c r="M187" s="12"/>
       <c r="N187" s="13"/>
     </row>
     <row r="188" spans="5:14">
-      <c r="E188" s="20" t="s">
+      <c r="E188" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F188" s="12"/>
+      <c r="G188" s="12"/>
+      <c r="H188" s="12"/>
+      <c r="I188" s="12"/>
+      <c r="J188" s="12"/>
+      <c r="K188" s="12"/>
+      <c r="L188" s="12"/>
+      <c r="M188" s="12"/>
+      <c r="N188" s="13"/>
+    </row>
+    <row r="189" spans="5:14">
+      <c r="E189" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F189" s="12"/>
+      <c r="G189" s="12"/>
+      <c r="H189" s="12"/>
+      <c r="I189" s="12"/>
+      <c r="J189" s="12"/>
+      <c r="K189" s="12"/>
+      <c r="L189" s="12"/>
+      <c r="M189" s="12"/>
+      <c r="N189" s="13"/>
+    </row>
+    <row r="190" spans="5:14">
+      <c r="E190" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F190" s="19"/>
+      <c r="G190" s="19"/>
+      <c r="H190" s="19"/>
+      <c r="I190" s="19"/>
+      <c r="J190" s="19"/>
+      <c r="K190" s="19"/>
+      <c r="L190" s="19"/>
+      <c r="M190" s="12"/>
+      <c r="N190" s="13"/>
+    </row>
+    <row r="191" spans="5:14">
+      <c r="E191" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F191" s="19"/>
+      <c r="G191" s="19"/>
+      <c r="H191" s="19"/>
+      <c r="I191" s="19"/>
+      <c r="J191" s="19"/>
+      <c r="K191" s="19"/>
+      <c r="L191" s="19"/>
+      <c r="M191" s="12"/>
+      <c r="N191" s="13"/>
+    </row>
+    <row r="192" spans="5:14">
+      <c r="E192" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F192" s="19"/>
+      <c r="G192" s="19"/>
+      <c r="H192" s="19"/>
+      <c r="I192" s="19"/>
+      <c r="J192" s="19"/>
+      <c r="K192" s="19"/>
+      <c r="L192" s="19"/>
+      <c r="M192" s="12"/>
+      <c r="N192" s="13"/>
+    </row>
+    <row r="193" spans="5:14">
+      <c r="E193" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F193" s="19"/>
+      <c r="G193" s="19"/>
+      <c r="H193" s="19"/>
+      <c r="I193" s="19"/>
+      <c r="J193" s="19"/>
+      <c r="K193" s="19"/>
+      <c r="L193" s="19"/>
+      <c r="M193" s="12"/>
+      <c r="N193" s="13"/>
+    </row>
+    <row r="194" spans="5:14">
+      <c r="E194" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F194" s="19"/>
+      <c r="G194" s="19"/>
+      <c r="H194" s="19"/>
+      <c r="I194" s="19"/>
+      <c r="J194" s="19"/>
+      <c r="K194" s="19"/>
+      <c r="L194" s="19"/>
+      <c r="M194" s="12"/>
+      <c r="N194" s="13"/>
+    </row>
+    <row r="195" spans="5:14">
+      <c r="E195" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F195" s="19"/>
+      <c r="G195" s="19"/>
+      <c r="H195" s="19"/>
+      <c r="I195" s="19"/>
+      <c r="J195" s="19"/>
+      <c r="K195" s="19"/>
+      <c r="L195" s="19"/>
+      <c r="M195" s="12"/>
+      <c r="N195" s="13"/>
+    </row>
+    <row r="196" spans="5:14">
+      <c r="E196" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="F188" s="21"/>
-      <c r="G188" s="21"/>
-      <c r="H188" s="21"/>
-      <c r="I188" s="21"/>
-      <c r="J188" s="21"/>
-      <c r="K188" s="21"/>
-      <c r="L188" s="21"/>
-      <c r="M188" s="15"/>
-      <c r="N188" s="16"/>
-    </row>
-    <row r="190" spans="5:14">
-      <c r="E190" s="5" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="191" spans="5:14">
-      <c r="E191" s="5" t="s">
+      <c r="F196" s="21"/>
+      <c r="G196" s="21"/>
+      <c r="H196" s="21"/>
+      <c r="I196" s="21"/>
+      <c r="J196" s="21"/>
+      <c r="K196" s="21"/>
+      <c r="L196" s="21"/>
+      <c r="M196" s="15"/>
+      <c r="N196" s="16"/>
+    </row>
+    <row r="198" spans="5:14">
+      <c r="E198" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="199" spans="5:14">
+      <c r="E199" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="192" spans="5:14">
-      <c r="E192" s="5" t="s">
+    <row r="200" spans="5:14">
+      <c r="E200" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="194" spans="3:5">
-      <c r="E194" s="5" t="s">
+    <row r="202" spans="5:14">
+      <c r="E202" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="195" spans="3:5">
-      <c r="E195" s="5" t="s">
+    <row r="203" spans="5:14">
+      <c r="E203" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="196" spans="3:5">
-      <c r="E196" s="5" t="s">
+    <row r="204" spans="5:14">
+      <c r="E204" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="197" spans="3:5">
-      <c r="E197" s="5" t="s">
+    <row r="205" spans="5:14">
+      <c r="E205" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="199" spans="3:5">
-      <c r="E199" s="5" t="s">
+    <row r="207" spans="5:14">
+      <c r="E207" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="200" spans="3:5">
-      <c r="E200" s="5" t="s">
+    <row r="208" spans="5:14">
+      <c r="E208" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="202" spans="3:5">
-      <c r="C202" s="24" t="s">
+    <row r="210" spans="3:5">
+      <c r="C210" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D210" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="212" spans="3:5">
+      <c r="D212" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E212" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="213" spans="3:5">
+      <c r="E213" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="214" spans="3:5">
+      <c r="D214" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E214" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="215" spans="3:5">
+      <c r="D215" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E215" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="216" spans="3:5">
+      <c r="E216" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="218" spans="3:5">
+      <c r="D218" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E218" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="219" spans="3:5">
+      <c r="E219" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="220" spans="3:5">
+      <c r="E220" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="221" spans="3:5">
+      <c r="E221" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="222" spans="3:5">
+      <c r="E222" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="223" spans="3:5">
+      <c r="E223" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="224" spans="3:5">
+      <c r="E224" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="227" spans="4:4">
+      <c r="D227" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D202" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="204" spans="3:5">
-      <c r="D204" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E204" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="205" spans="3:5">
-      <c r="E205" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="206" spans="3:5">
-      <c r="D206" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E206" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="207" spans="3:5">
-      <c r="D207" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E207" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="208" spans="3:5">
-      <c r="E208" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="210" spans="4:5">
-      <c r="D210" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E210" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="211" spans="4:5">
-      <c r="E211" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="212" spans="4:5">
-      <c r="E212" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="213" spans="4:5">
-      <c r="E213" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="214" spans="4:5">
-      <c r="E214" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="215" spans="4:5">
-      <c r="E215" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="216" spans="4:5">
-      <c r="E216" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="219" spans="4:5">
-      <c r="D219" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="220" spans="4:5">
-      <c r="D220" s="23"/>
-    </row>
-    <row r="247" spans="2:5">
-      <c r="B247" s="22">
+    </row>
+    <row r="228" spans="4:4">
+      <c r="D228" s="23"/>
+    </row>
+    <row r="255" spans="2:4">
+      <c r="B255" s="22">
         <v>3</v>
       </c>
-      <c r="C247" s="25" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="248" spans="2:5">
-      <c r="C248" s="24" t="s">
+      <c r="C255" s="25" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="256" spans="2:4">
+      <c r="C256" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="D256" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D248" s="5" t="s">
+    </row>
+    <row r="257" spans="4:5">
+      <c r="D257" s="5" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="249" spans="2:5">
-      <c r="D249" s="5" t="s">
+      <c r="E257" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="E249" s="5" t="s">
+    </row>
+    <row r="258" spans="4:5">
+      <c r="D258" s="5" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="250" spans="2:5">
-      <c r="D250" s="5" t="s">
+      <c r="E258" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="E250" s="5" t="s">
+    </row>
+    <row r="259" spans="4:5">
+      <c r="D259" s="5" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="251" spans="2:5">
-      <c r="D251" s="5" t="s">
+      <c r="E259" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="E251" s="5" t="s">
+    </row>
+    <row r="260" spans="4:5">
+      <c r="E260" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="252" spans="2:5">
-      <c r="E252" s="5" t="s">
+    <row r="261" spans="4:5">
+      <c r="E261" s="5" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="253" spans="2:5">
-      <c r="E253" s="5" t="s">
+    <row r="262" spans="4:5">
+      <c r="E262" s="5" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="254" spans="2:5">
-      <c r="E254" s="5" t="s">
+    <row r="263" spans="4:5">
+      <c r="E263" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="264" spans="4:5">
+      <c r="E264" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="265" spans="4:5">
+      <c r="E265" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="266" spans="4:5">
+      <c r="E266" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="267" spans="4:5">
+      <c r="E267" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="268" spans="4:5">
+      <c r="E268" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="269" spans="4:5">
+      <c r="E269" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="273" spans="3:5">
+      <c r="D273" s="5" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="255" spans="2:5">
-      <c r="E255" s="5" t="s">
+      <c r="E273" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="274" spans="3:5">
+      <c r="E274" s="5" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="256" spans="2:5">
-      <c r="E256" s="5" t="s">
+    <row r="275" spans="3:5">
+      <c r="E275" s="5" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="257" spans="2:5">
-      <c r="E257" s="5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="258" spans="2:5">
-      <c r="E258" s="5" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="259" spans="2:5">
-      <c r="E259" s="5" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="260" spans="2:5">
-      <c r="E260" s="5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="262" spans="2:5">
-      <c r="D262" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E262" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="263" spans="2:5">
-      <c r="E263" s="5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="264" spans="2:5">
-      <c r="E264" s="5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="266" spans="2:5">
-      <c r="B266" s="22">
+    <row r="277" spans="3:5">
+      <c r="C277" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="D277" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="278" spans="3:5">
+      <c r="D278" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="E278" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="279" spans="3:5">
+      <c r="D279" s="5">
+        <v>1</v>
+      </c>
+      <c r="E279" s="6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="280" spans="3:5">
+      <c r="E280" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="281" spans="3:5">
+      <c r="E281" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="282" spans="3:5">
+      <c r="E282" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="283" spans="3:5">
+      <c r="E283" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="285" spans="3:5">
+      <c r="D285" s="5">
+        <v>2</v>
+      </c>
+      <c r="E285" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="286" spans="3:5">
+      <c r="E286" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="287" spans="3:5">
+      <c r="E287" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="288" spans="3:5">
+      <c r="E288" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="289" spans="2:5">
+      <c r="E289" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="295" spans="2:5">
+      <c r="B295" s="22">
         <v>4</v>
       </c>
-      <c r="C266" s="24" t="s">
-        <v>284</v>
+      <c r="C295" s="24" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -4067,7 +4256,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -4075,7 +4264,7 @@
         <v>119</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -4083,7 +4272,7 @@
         <v>117</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -4124,7 +4313,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4132,31 +4321,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="C6" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4164,12 +4353,12 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="D8" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4177,30 +4366,30 @@
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="D10" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="D11" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="D13" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="B26" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -4208,26 +4397,26 @@
         <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="B29" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -4263,7 +4452,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4271,20 +4460,20 @@
         <v>117</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="C4" s="1" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" s="1" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4292,25 +4481,25 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="C9" s="5"/>
       <c r="D9" s="2" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4321,43 +4510,43 @@
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="D13" s="1" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="D14" s="1" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="D15" s="2" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="D16" s="1" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32" spans="4:4">
       <c r="D32" s="1" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="1" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Date:2016-04-09 Description：NoteBook.xlsx完善git的学习              git add -u;              git rm; git rm -n; git rm --cached;              git config alias.st status;git config --unset alias.st;              git config commit.template templatefile.txt;              .gitignore;              vim光标移到文件开头/文件结尾:冒号1==>开头;冒号$==>结尾;
</commit_message>
<xml_diff>
--- a/NoteBook.xlsx
+++ b/NoteBook.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="目录" sheetId="1" r:id="rId1"/>
-    <sheet name="宏的使用" sheetId="2" r:id="rId2"/>
-    <sheet name="Git的使用" sheetId="3" r:id="rId3"/>
+    <sheet name="Git的使用" sheetId="3" r:id="rId2"/>
+    <sheet name="宏的使用" sheetId="2" r:id="rId3"/>
     <sheet name="Mac使用技巧" sheetId="4" r:id="rId4"/>
     <sheet name="Xcode调试常见问题" sheetId="5" r:id="rId5"/>
     <sheet name="Excel使用技巧" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Git_管理本地仓库">Git的使用!$C$17</definedName>
-    <definedName name="Git_配置">Git的使用!$C$255</definedName>
-    <definedName name="Git_与远程主机的交互">Git的使用!$C$128</definedName>
+    <definedName name="Git_配置">Git的使用!$C$274</definedName>
+    <definedName name="Git_与远程主机的交互">Git的使用!$C$147</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="334">
   <si>
     <t>#else</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1350,27 +1350,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>在弹出的框框中的"在工作簿中的名称"输入框输入名称,如"Git_分支管理"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Git_分支管理</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>这种链接,点击某单元格最终会链接到"Git的使用"工作表,且焦点单元格是左上角</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>选中单元格-&gt;工具栏中的"插入"-&gt;"名称"-&gt;"定义"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>右键"Git的使用"单元格-&gt;"超链接"-&gt;"文档"-&gt;"查找"-&gt;在列表中选择工作表"Git的使用"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2-2 在点击的单元(任意单元格)"右键"-&gt;"超链接"-&gt;"文档"-&gt;"查找"-&gt;"已定义的名称"-&gt;选择你之前定义的名称"Git_分支管理"</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1569,6 +1553,192 @@
   </si>
   <si>
     <t>交互式的添加</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git commit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git diff</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git rm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git rm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除文件操作</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用法</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git rm temp.txt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除temp.txt文件,worksapce和local repo中该文件都将被删除</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git rm -n temp.txt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>这个命令会确认要删除的文件,即,命令不会做出删除文件的操作,只是列出来,以便做确认,以免误删</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>待确认完之后,可以采用上面1的命令做真正的删除操作</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git rm --cached temp.txt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除local repo中该文件,但workspace中保留,即只是从版本管理中移除该文件而已</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>因为有时候,我们可能提交了很多文件,但是其中的某些文件并不需要版本管理的,</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>可是这些文件却又需要在工作目录中保留,则可以选择只从版本库中移除,本地保留即可.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>这种情况下,每次git status则会提示这些文件Untracked..如果觉得也不需要这些提示,</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>那么可以在.gitignore中配置忽略这些文件.git status 就显示clean了</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>别忘了,git rm  之后,还是要commit的!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    选中单元格-&gt;工具栏中的"插入"-&gt;"名称"-&gt;"定义"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>效果:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>点击某单元格最终会链接到"Git的使用"工作表,且焦点单元格是左上角</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    在弹出的框框中的"在工作簿中的名称"输入框</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>输入名称</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,如"Git_分支管理"</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-2 做超链接</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>选中单元格</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(任意)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"右键"-&gt;"超链接"-&gt;"文档"-&gt;"查找"-&gt;"已定义的名称"-&gt;选择已定义的名称</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Git_分支管理"</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Object-C</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1756,7 +1926,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1793,6 +1963,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1878,7 +2051,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="35" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="54">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -1929,6 +2102,9 @@
     <cellStyle name="访问过的超链接" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1942,13 +2118,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>227</xdr:row>
+      <xdr:row>246</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>251</xdr:row>
+      <xdr:row>270</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2458,9 +2634,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D23"/>
+  <dimension ref="B3:D24"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A5" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0"/>
   <cols>
@@ -2476,84 +2652,92 @@
       </c>
     </row>
     <row r="4" spans="2:4">
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="C5" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="2:4">
+      <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="1">
+    <row r="12" spans="2:4">
+      <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
-      <c r="C12" s="3" t="s">
+    <row r="13" spans="2:4">
+      <c r="C13" s="3" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="D13" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="D14" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="D15" s="1" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="1">
         <v>3</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="1" t="s">
+    <row r="21" spans="2:4">
+      <c r="B21" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="1">
+    <row r="22" spans="2:4">
+      <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
-      <c r="C22" s="3" t="s">
+    <row r="23" spans="2:4">
+      <c r="C23" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
-      <c r="D23" s="1" t="s">
+    <row r="24" spans="2:4">
+      <c r="D24" s="1" t="s">
         <v>180</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C4" location="宏的使用!A1" tooltip="宏的使用" display="宏的使用"/>
-    <hyperlink ref="C15" location="Git的使用!A1" tooltip="Git" display="Git"/>
-    <hyperlink ref="C22" location="Mac使用技巧!A1" tooltip="常用小技巧" display="使用技巧"/>
-    <hyperlink ref="C12" location="Xcode调试常见问题!A1" tooltip="Xcode调试常见异常信息" display="调试常见问题"/>
+    <hyperlink ref="C5" location="宏的使用!A1" tooltip="宏的使用" display="宏的使用"/>
+    <hyperlink ref="C16" location="Git的使用!A1" tooltip="Git" display="Git"/>
+    <hyperlink ref="C23" location="Mac使用技巧!A1" tooltip="常用小技巧" display="使用技巧"/>
+    <hyperlink ref="C13" location="Xcode调试常见问题!A1" tooltip="Xcode调试常见异常信息" display="调试常见问题"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2566,6 +2750,1510 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N314"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="D141" sqref="D141"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="22"/>
+    <col min="3" max="3" width="12.1640625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" s="24"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" s="3"/>
+      <c r="C9" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" s="3"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" s="24"/>
+      <c r="C14" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="22">
+        <v>1</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="C18" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="D19" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="D20" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="D21" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="E22" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="E23" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="E24" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="D25" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="E26" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="E28" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="E29" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="E30" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="E32" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5">
+      <c r="E33" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5">
+      <c r="D36" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5">
+      <c r="E37" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5">
+      <c r="C39" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5">
+      <c r="D40" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5">
+      <c r="D41" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5">
+      <c r="E42" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5">
+      <c r="D44" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5">
+      <c r="E45" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5">
+      <c r="E46" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5">
+      <c r="E47" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5">
+      <c r="E48" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="49" spans="4:13">
+      <c r="E49" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="4:13">
+      <c r="E50" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="52" spans="4:13">
+      <c r="D52" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="53" spans="4:13">
+      <c r="E53" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="54" spans="4:13">
+      <c r="E54" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="55" spans="4:13">
+      <c r="E55" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="56" spans="4:13">
+      <c r="E56" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="60" spans="4:13">
+      <c r="D60" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="M60" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="88" spans="3:6">
+      <c r="C88" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6">
+      <c r="D89" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="90" spans="3:6">
+      <c r="D90" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="91" spans="3:6">
+      <c r="E91" s="5">
+        <v>1</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="92" spans="3:6">
+      <c r="F92" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="94" spans="3:6">
+      <c r="E94" s="5">
+        <v>2</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="95" spans="3:6">
+      <c r="F95" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="97" spans="4:6">
+      <c r="E97" s="5">
+        <v>3</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="98" spans="4:6">
+      <c r="F98" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6">
+      <c r="D100" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6">
+      <c r="E101" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="102" spans="4:6">
+      <c r="E102" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="103" spans="4:6">
+      <c r="E103" s="5">
+        <v>1</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="104" spans="4:6">
+      <c r="F104" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="105" spans="4:6">
+      <c r="E105" s="5">
+        <v>2</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="106" spans="4:6">
+      <c r="F106" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="107" spans="4:6">
+      <c r="F107" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="4:6">
+      <c r="F108" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="109" spans="4:6">
+      <c r="F109" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="110" spans="4:6">
+      <c r="F110" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="111" spans="4:6">
+      <c r="E111" s="5">
+        <v>3</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="112" spans="4:6">
+      <c r="F112" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="113" spans="3:6">
+      <c r="F113" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="114" spans="3:6">
+      <c r="F114" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="115" spans="3:6">
+      <c r="E115" s="5">
+        <v>4</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="116" spans="3:6">
+      <c r="F116" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="117" spans="3:6">
+      <c r="F117" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="118" spans="3:6">
+      <c r="F118" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="119" spans="3:6">
+      <c r="E119" s="5">
+        <v>5</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="120" spans="3:6">
+      <c r="F120" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="121" spans="3:6">
+      <c r="F121" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="122" spans="3:6">
+      <c r="F122" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="123" spans="3:6">
+      <c r="F123" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="124" spans="3:6">
+      <c r="E124" s="5">
+        <v>6</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="127" spans="3:6">
+      <c r="C127" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="128" spans="3:6">
+      <c r="D128" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="129" spans="4:5">
+      <c r="D129" s="5" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="130" spans="4:5">
+      <c r="D130" s="5">
+        <v>1</v>
+      </c>
+      <c r="E130" s="6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="131" spans="4:5">
+      <c r="E131" s="5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="133" spans="4:5">
+      <c r="D133" s="5">
+        <v>2</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="134" spans="4:5">
+      <c r="E134" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="135" spans="4:5">
+      <c r="E135" s="5" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="137" spans="4:5">
+      <c r="D137" s="5">
+        <v>3</v>
+      </c>
+      <c r="E137" s="6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="138" spans="4:5">
+      <c r="E138" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="139" spans="4:5">
+      <c r="E139" s="5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="140" spans="4:5">
+      <c r="E140" s="5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="141" spans="4:5">
+      <c r="E141" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="142" spans="4:5">
+      <c r="E142" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="144" spans="4:5">
+      <c r="D144" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="E144" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5">
+      <c r="B147" s="22">
+        <v>2</v>
+      </c>
+      <c r="C147" s="25" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5">
+      <c r="C148" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5">
+      <c r="D150" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E150" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5">
+      <c r="D151" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E151" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5">
+      <c r="D152" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E152" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5">
+      <c r="E153" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="155" spans="2:5">
+      <c r="E155" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="156" spans="2:5">
+      <c r="E156" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="157" spans="2:5">
+      <c r="E157" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="159" spans="2:5">
+      <c r="C159" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D159" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="161" spans="3:12">
+      <c r="D161" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E161" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="162" spans="3:12">
+      <c r="D162" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E162" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="163" spans="3:12">
+      <c r="E163" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F163" s="9"/>
+      <c r="G163" s="9"/>
+      <c r="H163" s="9"/>
+      <c r="I163" s="9"/>
+      <c r="J163" s="9"/>
+      <c r="K163" s="10"/>
+    </row>
+    <row r="164" spans="3:12">
+      <c r="E164" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F164" s="12"/>
+      <c r="G164" s="12"/>
+      <c r="H164" s="12"/>
+      <c r="I164" s="12"/>
+      <c r="J164" s="12"/>
+      <c r="K164" s="13"/>
+    </row>
+    <row r="165" spans="3:12">
+      <c r="E165" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F165" s="12"/>
+      <c r="G165" s="12"/>
+      <c r="H165" s="12"/>
+      <c r="I165" s="12"/>
+      <c r="J165" s="12"/>
+      <c r="K165" s="13"/>
+    </row>
+    <row r="166" spans="3:12">
+      <c r="E166" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F166" s="15"/>
+      <c r="G166" s="15"/>
+      <c r="H166" s="15"/>
+      <c r="I166" s="15"/>
+      <c r="J166" s="15"/>
+      <c r="K166" s="16"/>
+    </row>
+    <row r="168" spans="3:12">
+      <c r="E168" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="169" spans="3:12">
+      <c r="E169" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F169" s="9"/>
+      <c r="G169" s="9"/>
+      <c r="H169" s="9"/>
+      <c r="I169" s="9"/>
+      <c r="J169" s="9"/>
+      <c r="K169" s="9"/>
+      <c r="L169" s="10"/>
+    </row>
+    <row r="170" spans="3:12">
+      <c r="E170" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F170" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="G170" s="12"/>
+      <c r="H170" s="12"/>
+      <c r="I170" s="12"/>
+      <c r="J170" s="12"/>
+      <c r="K170" s="12"/>
+      <c r="L170" s="13"/>
+    </row>
+    <row r="171" spans="3:12">
+      <c r="E171" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F171" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G171" s="15"/>
+      <c r="H171" s="15"/>
+      <c r="I171" s="15"/>
+      <c r="J171" s="15"/>
+      <c r="K171" s="15"/>
+      <c r="L171" s="16"/>
+    </row>
+    <row r="173" spans="3:12">
+      <c r="C173" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D173" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="175" spans="3:12">
+      <c r="D175" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E175" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="176" spans="3:12">
+      <c r="D176" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E176" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="177" spans="3:5">
+      <c r="E177" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="178" spans="3:5">
+      <c r="D178" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E178" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="179" spans="3:5">
+      <c r="E179" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="180" spans="3:5">
+      <c r="E180" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="181" spans="3:5">
+      <c r="E181" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="182" spans="3:5">
+      <c r="E182" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="183" spans="3:5">
+      <c r="E183" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="184" spans="3:5">
+      <c r="E184" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="186" spans="3:5">
+      <c r="C186" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D186" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="188" spans="3:5">
+      <c r="D188" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E188" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="189" spans="3:5">
+      <c r="D189" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E189" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="190" spans="3:5">
+      <c r="D190" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E190" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="191" spans="3:5">
+      <c r="E191" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="192" spans="3:5">
+      <c r="E192" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="195" spans="4:14">
+      <c r="D195" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E195" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="196" spans="4:14">
+      <c r="E196" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="197" spans="4:14">
+      <c r="E197" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F197" s="9"/>
+      <c r="G197" s="9"/>
+      <c r="H197" s="9"/>
+      <c r="I197" s="9"/>
+      <c r="J197" s="9"/>
+      <c r="K197" s="9"/>
+      <c r="L197" s="9"/>
+      <c r="M197" s="9"/>
+      <c r="N197" s="10"/>
+    </row>
+    <row r="198" spans="4:14">
+      <c r="E198" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F198" s="12"/>
+      <c r="G198" s="12"/>
+      <c r="H198" s="12"/>
+      <c r="I198" s="12"/>
+      <c r="J198" s="12"/>
+      <c r="K198" s="12"/>
+      <c r="L198" s="12"/>
+      <c r="M198" s="12"/>
+      <c r="N198" s="13"/>
+    </row>
+    <row r="199" spans="4:14">
+      <c r="E199" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F199" s="12"/>
+      <c r="G199" s="12"/>
+      <c r="H199" s="12"/>
+      <c r="I199" s="12"/>
+      <c r="J199" s="12"/>
+      <c r="K199" s="12"/>
+      <c r="L199" s="12"/>
+      <c r="M199" s="12"/>
+      <c r="N199" s="13"/>
+    </row>
+    <row r="200" spans="4:14">
+      <c r="E200" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F200" s="12"/>
+      <c r="G200" s="12"/>
+      <c r="H200" s="12"/>
+      <c r="I200" s="12"/>
+      <c r="J200" s="12"/>
+      <c r="K200" s="12"/>
+      <c r="L200" s="12"/>
+      <c r="M200" s="12"/>
+      <c r="N200" s="13"/>
+    </row>
+    <row r="201" spans="4:14">
+      <c r="E201" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F201" s="12"/>
+      <c r="G201" s="12"/>
+      <c r="H201" s="12"/>
+      <c r="I201" s="12"/>
+      <c r="J201" s="12"/>
+      <c r="K201" s="12"/>
+      <c r="L201" s="12"/>
+      <c r="M201" s="12"/>
+      <c r="N201" s="13"/>
+    </row>
+    <row r="202" spans="4:14">
+      <c r="E202" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F202" s="12"/>
+      <c r="G202" s="12"/>
+      <c r="H202" s="12"/>
+      <c r="I202" s="12"/>
+      <c r="J202" s="12"/>
+      <c r="K202" s="12"/>
+      <c r="L202" s="12"/>
+      <c r="M202" s="12"/>
+      <c r="N202" s="13"/>
+    </row>
+    <row r="203" spans="4:14">
+      <c r="E203" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F203" s="12"/>
+      <c r="G203" s="12"/>
+      <c r="H203" s="12"/>
+      <c r="I203" s="12"/>
+      <c r="J203" s="12"/>
+      <c r="K203" s="12"/>
+      <c r="L203" s="12"/>
+      <c r="M203" s="12"/>
+      <c r="N203" s="13"/>
+    </row>
+    <row r="204" spans="4:14">
+      <c r="E204" s="11"/>
+      <c r="F204" s="12"/>
+      <c r="G204" s="12"/>
+      <c r="H204" s="12"/>
+      <c r="I204" s="12"/>
+      <c r="J204" s="12"/>
+      <c r="K204" s="12"/>
+      <c r="L204" s="12"/>
+      <c r="M204" s="12"/>
+      <c r="N204" s="13"/>
+    </row>
+    <row r="205" spans="4:14">
+      <c r="E205" s="11"/>
+      <c r="F205" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G205" s="12"/>
+      <c r="H205" s="12"/>
+      <c r="I205" s="12"/>
+      <c r="J205" s="12"/>
+      <c r="K205" s="12"/>
+      <c r="L205" s="12"/>
+      <c r="M205" s="12"/>
+      <c r="N205" s="13"/>
+    </row>
+    <row r="206" spans="4:14">
+      <c r="E206" s="11"/>
+      <c r="F206" s="12"/>
+      <c r="G206" s="12"/>
+      <c r="H206" s="12"/>
+      <c r="I206" s="12"/>
+      <c r="J206" s="12"/>
+      <c r="K206" s="12"/>
+      <c r="L206" s="12"/>
+      <c r="M206" s="12"/>
+      <c r="N206" s="13"/>
+    </row>
+    <row r="207" spans="4:14">
+      <c r="E207" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F207" s="12"/>
+      <c r="G207" s="12"/>
+      <c r="H207" s="12"/>
+      <c r="I207" s="12"/>
+      <c r="J207" s="12"/>
+      <c r="K207" s="12"/>
+      <c r="L207" s="12"/>
+      <c r="M207" s="12"/>
+      <c r="N207" s="13"/>
+    </row>
+    <row r="208" spans="4:14">
+      <c r="E208" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F208" s="12"/>
+      <c r="G208" s="12"/>
+      <c r="H208" s="12"/>
+      <c r="I208" s="12"/>
+      <c r="J208" s="12"/>
+      <c r="K208" s="12"/>
+      <c r="L208" s="12"/>
+      <c r="M208" s="12"/>
+      <c r="N208" s="13"/>
+    </row>
+    <row r="209" spans="5:14">
+      <c r="E209" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F209" s="19"/>
+      <c r="G209" s="19"/>
+      <c r="H209" s="19"/>
+      <c r="I209" s="19"/>
+      <c r="J209" s="19"/>
+      <c r="K209" s="19"/>
+      <c r="L209" s="19"/>
+      <c r="M209" s="12"/>
+      <c r="N209" s="13"/>
+    </row>
+    <row r="210" spans="5:14">
+      <c r="E210" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F210" s="19"/>
+      <c r="G210" s="19"/>
+      <c r="H210" s="19"/>
+      <c r="I210" s="19"/>
+      <c r="J210" s="19"/>
+      <c r="K210" s="19"/>
+      <c r="L210" s="19"/>
+      <c r="M210" s="12"/>
+      <c r="N210" s="13"/>
+    </row>
+    <row r="211" spans="5:14">
+      <c r="E211" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F211" s="19"/>
+      <c r="G211" s="19"/>
+      <c r="H211" s="19"/>
+      <c r="I211" s="19"/>
+      <c r="J211" s="19"/>
+      <c r="K211" s="19"/>
+      <c r="L211" s="19"/>
+      <c r="M211" s="12"/>
+      <c r="N211" s="13"/>
+    </row>
+    <row r="212" spans="5:14">
+      <c r="E212" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F212" s="19"/>
+      <c r="G212" s="19"/>
+      <c r="H212" s="19"/>
+      <c r="I212" s="19"/>
+      <c r="J212" s="19"/>
+      <c r="K212" s="19"/>
+      <c r="L212" s="19"/>
+      <c r="M212" s="12"/>
+      <c r="N212" s="13"/>
+    </row>
+    <row r="213" spans="5:14">
+      <c r="E213" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F213" s="19"/>
+      <c r="G213" s="19"/>
+      <c r="H213" s="19"/>
+      <c r="I213" s="19"/>
+      <c r="J213" s="19"/>
+      <c r="K213" s="19"/>
+      <c r="L213" s="19"/>
+      <c r="M213" s="12"/>
+      <c r="N213" s="13"/>
+    </row>
+    <row r="214" spans="5:14">
+      <c r="E214" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F214" s="19"/>
+      <c r="G214" s="19"/>
+      <c r="H214" s="19"/>
+      <c r="I214" s="19"/>
+      <c r="J214" s="19"/>
+      <c r="K214" s="19"/>
+      <c r="L214" s="19"/>
+      <c r="M214" s="12"/>
+      <c r="N214" s="13"/>
+    </row>
+    <row r="215" spans="5:14">
+      <c r="E215" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F215" s="21"/>
+      <c r="G215" s="21"/>
+      <c r="H215" s="21"/>
+      <c r="I215" s="21"/>
+      <c r="J215" s="21"/>
+      <c r="K215" s="21"/>
+      <c r="L215" s="21"/>
+      <c r="M215" s="15"/>
+      <c r="N215" s="16"/>
+    </row>
+    <row r="217" spans="5:14">
+      <c r="E217" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="218" spans="5:14">
+      <c r="E218" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="219" spans="5:14">
+      <c r="E219" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="221" spans="5:14">
+      <c r="E221" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="222" spans="5:14">
+      <c r="E222" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="223" spans="5:14">
+      <c r="E223" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="224" spans="5:14">
+      <c r="E224" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="226" spans="3:5">
+      <c r="E226" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="227" spans="3:5">
+      <c r="E227" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="229" spans="3:5">
+      <c r="C229" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D229" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="231" spans="3:5">
+      <c r="D231" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E231" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="232" spans="3:5">
+      <c r="E232" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="233" spans="3:5">
+      <c r="D233" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E233" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="234" spans="3:5">
+      <c r="D234" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E234" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="235" spans="3:5">
+      <c r="E235" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="237" spans="3:5">
+      <c r="D237" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E237" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="238" spans="3:5">
+      <c r="E238" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="239" spans="3:5">
+      <c r="E239" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="240" spans="3:5">
+      <c r="E240" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="241" spans="4:5">
+      <c r="E241" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="242" spans="4:5">
+      <c r="E242" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="243" spans="4:5">
+      <c r="E243" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="246" spans="4:5">
+      <c r="D246" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="247" spans="4:5">
+      <c r="D247" s="23"/>
+    </row>
+    <row r="274" spans="2:5">
+      <c r="B274" s="22">
+        <v>3</v>
+      </c>
+      <c r="C274" s="25" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="275" spans="2:5">
+      <c r="C275" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="D275" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="276" spans="2:5">
+      <c r="D276" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="E276" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="277" spans="2:5">
+      <c r="D277" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E277" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="278" spans="2:5">
+      <c r="D278" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E278" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="279" spans="2:5">
+      <c r="E279" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="280" spans="2:5">
+      <c r="E280" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="281" spans="2:5">
+      <c r="E281" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="282" spans="2:5">
+      <c r="E282" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="283" spans="2:5">
+      <c r="E283" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="284" spans="2:5">
+      <c r="E284" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="285" spans="2:5">
+      <c r="E285" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="286" spans="2:5">
+      <c r="E286" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="287" spans="2:5">
+      <c r="E287" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="288" spans="2:5">
+      <c r="E288" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="292" spans="3:5">
+      <c r="D292" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="E292" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="293" spans="3:5">
+      <c r="E293" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="294" spans="3:5">
+      <c r="E294" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="296" spans="3:5">
+      <c r="C296" s="24" t="s">
+        <v>279</v>
+      </c>
+      <c r="D296" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="297" spans="3:5">
+      <c r="D297" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E297" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="298" spans="3:5">
+      <c r="D298" s="5">
+        <v>1</v>
+      </c>
+      <c r="E298" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="299" spans="3:5">
+      <c r="E299" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="300" spans="3:5">
+      <c r="E300" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="301" spans="3:5">
+      <c r="E301" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="302" spans="3:5">
+      <c r="E302" s="6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="304" spans="3:5">
+      <c r="D304" s="5">
+        <v>2</v>
+      </c>
+      <c r="E304" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="305" spans="2:5">
+      <c r="E305" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="306" spans="2:5">
+      <c r="E306" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="307" spans="2:5">
+      <c r="E307" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="308" spans="2:5">
+      <c r="E308" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="314" spans="2:5">
+      <c r="B314" s="22">
+        <v>4</v>
+      </c>
+      <c r="C314" s="24" t="s">
+        <v>275</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" location="目录!A1" tooltip="返回目录" display="返回"/>
+    <hyperlink ref="B12" location="Git_与远程主机的交互" tooltip="Git_与远程主机的交互" display="与远程仓库交互"/>
+    <hyperlink ref="B6" location="Git_管理本地仓库" tooltip="Git_管理本地仓库" display="管理本地仓库"/>
+    <hyperlink ref="B13" location="Git_配置" tooltip="Git_配置" display="git配置"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F57"/>
   <sheetViews>
@@ -2829,1411 +4517,6 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N295"/>
-  <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="22"/>
-    <col min="3" max="3" width="12.1640625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="B2" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="25" t="s">
-        <v>234</v>
-      </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="24"/>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" s="3"/>
-      <c r="C7" s="5" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" s="3"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" s="3"/>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" s="3"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="B13" s="26" t="s">
-        <v>255</v>
-      </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" s="24"/>
-      <c r="C14" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="22">
-        <v>1</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="C18" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="D19" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="D20" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="D21" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="E22" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="E23" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="E24" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="D25" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="E26" s="5" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="E28" s="6" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="E29" s="5" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="E30" s="5" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5">
-      <c r="E32" s="5" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5">
-      <c r="E33" s="5" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5">
-      <c r="D36" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5">
-      <c r="E37" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="3:5">
-      <c r="C39" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="3:5">
-      <c r="D40" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5">
-      <c r="D41" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="42" spans="3:5">
-      <c r="E42" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="44" spans="3:5">
-      <c r="D44" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="45" spans="3:5">
-      <c r="E45" s="5" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="46" spans="3:5">
-      <c r="E46" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="47" spans="3:5">
-      <c r="E47" s="5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="48" spans="3:5">
-      <c r="E48" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="49" spans="4:13">
-      <c r="E49" s="5" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="50" spans="4:13">
-      <c r="E50" s="5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="52" spans="4:13">
-      <c r="D52" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="53" spans="4:13">
-      <c r="E53" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="54" spans="4:13">
-      <c r="E54" s="6" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="55" spans="4:13">
-      <c r="E55" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="56" spans="4:13">
-      <c r="E56" s="5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="60" spans="4:13">
-      <c r="D60" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="M60" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="88" spans="3:6">
-      <c r="C88" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="89" spans="3:6">
-      <c r="D89" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="90" spans="3:6">
-      <c r="D90" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="91" spans="3:6">
-      <c r="E91" s="5">
-        <v>1</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="92" spans="3:6">
-      <c r="F92" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="94" spans="3:6">
-      <c r="E94" s="5">
-        <v>2</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="95" spans="3:6">
-      <c r="F95" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="97" spans="4:6">
-      <c r="E97" s="5">
-        <v>3</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="98" spans="4:6">
-      <c r="F98" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="100" spans="4:6">
-      <c r="D100" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="101" spans="4:6">
-      <c r="E101" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="102" spans="4:6">
-      <c r="E102" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="103" spans="4:6">
-      <c r="E103" s="5">
-        <v>1</v>
-      </c>
-      <c r="F103" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="104" spans="4:6">
-      <c r="F104" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="105" spans="4:6">
-      <c r="E105" s="5">
-        <v>2</v>
-      </c>
-      <c r="F105" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="106" spans="4:6">
-      <c r="F106" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="107" spans="4:6">
-      <c r="F107" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="108" spans="4:6">
-      <c r="F108" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="109" spans="4:6">
-      <c r="F109" s="5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="110" spans="4:6">
-      <c r="F110" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="111" spans="4:6">
-      <c r="E111" s="5">
-        <v>3</v>
-      </c>
-      <c r="F111" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="112" spans="4:6">
-      <c r="F112" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6">
-      <c r="F113" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6">
-      <c r="F114" s="5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="115" spans="2:6">
-      <c r="E115" s="5">
-        <v>4</v>
-      </c>
-      <c r="F115" s="5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="116" spans="2:6">
-      <c r="F116" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="117" spans="2:6">
-      <c r="F117" s="5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="118" spans="2:6">
-      <c r="F118" s="5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="119" spans="2:6">
-      <c r="E119" s="5">
-        <v>5</v>
-      </c>
-      <c r="F119" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6">
-      <c r="F120" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6">
-      <c r="F121" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="122" spans="2:6">
-      <c r="F122" s="5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6">
-      <c r="F123" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6">
-      <c r="E124" s="5">
-        <v>6</v>
-      </c>
-      <c r="F124" s="5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="128" spans="2:6">
-      <c r="B128" s="22">
-        <v>2</v>
-      </c>
-      <c r="C128" s="25" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="129" spans="3:11">
-      <c r="C129" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D129" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="131" spans="3:11">
-      <c r="D131" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E131" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="132" spans="3:11">
-      <c r="D132" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E132" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="133" spans="3:11">
-      <c r="D133" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E133" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="134" spans="3:11">
-      <c r="E134" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="136" spans="3:11">
-      <c r="E136" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="137" spans="3:11">
-      <c r="E137" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="138" spans="3:11">
-      <c r="E138" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="140" spans="3:11">
-      <c r="C140" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="D140" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="142" spans="3:11">
-      <c r="D142" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E142" s="5" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="143" spans="3:11">
-      <c r="D143" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E143" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="144" spans="3:11">
-      <c r="E144" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F144" s="9"/>
-      <c r="G144" s="9"/>
-      <c r="H144" s="9"/>
-      <c r="I144" s="9"/>
-      <c r="J144" s="9"/>
-      <c r="K144" s="10"/>
-    </row>
-    <row r="145" spans="3:12">
-      <c r="E145" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F145" s="12"/>
-      <c r="G145" s="12"/>
-      <c r="H145" s="12"/>
-      <c r="I145" s="12"/>
-      <c r="J145" s="12"/>
-      <c r="K145" s="13"/>
-    </row>
-    <row r="146" spans="3:12">
-      <c r="E146" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F146" s="12"/>
-      <c r="G146" s="12"/>
-      <c r="H146" s="12"/>
-      <c r="I146" s="12"/>
-      <c r="J146" s="12"/>
-      <c r="K146" s="13"/>
-    </row>
-    <row r="147" spans="3:12">
-      <c r="E147" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F147" s="15"/>
-      <c r="G147" s="15"/>
-      <c r="H147" s="15"/>
-      <c r="I147" s="15"/>
-      <c r="J147" s="15"/>
-      <c r="K147" s="16"/>
-    </row>
-    <row r="149" spans="3:12">
-      <c r="E149" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="150" spans="3:12">
-      <c r="E150" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F150" s="9"/>
-      <c r="G150" s="9"/>
-      <c r="H150" s="9"/>
-      <c r="I150" s="9"/>
-      <c r="J150" s="9"/>
-      <c r="K150" s="9"/>
-      <c r="L150" s="10"/>
-    </row>
-    <row r="151" spans="3:12">
-      <c r="E151" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F151" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="G151" s="12"/>
-      <c r="H151" s="12"/>
-      <c r="I151" s="12"/>
-      <c r="J151" s="12"/>
-      <c r="K151" s="12"/>
-      <c r="L151" s="13"/>
-    </row>
-    <row r="152" spans="3:12">
-      <c r="E152" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F152" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G152" s="15"/>
-      <c r="H152" s="15"/>
-      <c r="I152" s="15"/>
-      <c r="J152" s="15"/>
-      <c r="K152" s="15"/>
-      <c r="L152" s="16"/>
-    </row>
-    <row r="154" spans="3:12">
-      <c r="C154" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="D154" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="156" spans="3:12">
-      <c r="D156" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E156" s="5" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="157" spans="3:12">
-      <c r="D157" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E157" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="158" spans="3:12">
-      <c r="E158" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="159" spans="3:12">
-      <c r="D159" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E159" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="160" spans="3:12">
-      <c r="E160" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="161" spans="3:5">
-      <c r="E161" s="5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="162" spans="3:5">
-      <c r="E162" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="163" spans="3:5">
-      <c r="E163" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="164" spans="3:5">
-      <c r="E164" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="165" spans="3:5">
-      <c r="E165" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="167" spans="3:5">
-      <c r="C167" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="D167" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="169" spans="3:5">
-      <c r="D169" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E169" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="170" spans="3:5">
-      <c r="D170" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E170" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="171" spans="3:5">
-      <c r="D171" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E171" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="172" spans="3:5">
-      <c r="E172" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="173" spans="3:5">
-      <c r="E173" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="176" spans="3:5">
-      <c r="D176" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E176" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="177" spans="5:14">
-      <c r="E177" s="5" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="178" spans="5:14">
-      <c r="E178" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F178" s="9"/>
-      <c r="G178" s="9"/>
-      <c r="H178" s="9"/>
-      <c r="I178" s="9"/>
-      <c r="J178" s="9"/>
-      <c r="K178" s="9"/>
-      <c r="L178" s="9"/>
-      <c r="M178" s="9"/>
-      <c r="N178" s="10"/>
-    </row>
-    <row r="179" spans="5:14">
-      <c r="E179" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F179" s="12"/>
-      <c r="G179" s="12"/>
-      <c r="H179" s="12"/>
-      <c r="I179" s="12"/>
-      <c r="J179" s="12"/>
-      <c r="K179" s="12"/>
-      <c r="L179" s="12"/>
-      <c r="M179" s="12"/>
-      <c r="N179" s="13"/>
-    </row>
-    <row r="180" spans="5:14">
-      <c r="E180" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F180" s="12"/>
-      <c r="G180" s="12"/>
-      <c r="H180" s="12"/>
-      <c r="I180" s="12"/>
-      <c r="J180" s="12"/>
-      <c r="K180" s="12"/>
-      <c r="L180" s="12"/>
-      <c r="M180" s="12"/>
-      <c r="N180" s="13"/>
-    </row>
-    <row r="181" spans="5:14">
-      <c r="E181" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F181" s="12"/>
-      <c r="G181" s="12"/>
-      <c r="H181" s="12"/>
-      <c r="I181" s="12"/>
-      <c r="J181" s="12"/>
-      <c r="K181" s="12"/>
-      <c r="L181" s="12"/>
-      <c r="M181" s="12"/>
-      <c r="N181" s="13"/>
-    </row>
-    <row r="182" spans="5:14">
-      <c r="E182" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F182" s="12"/>
-      <c r="G182" s="12"/>
-      <c r="H182" s="12"/>
-      <c r="I182" s="12"/>
-      <c r="J182" s="12"/>
-      <c r="K182" s="12"/>
-      <c r="L182" s="12"/>
-      <c r="M182" s="12"/>
-      <c r="N182" s="13"/>
-    </row>
-    <row r="183" spans="5:14">
-      <c r="E183" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F183" s="12"/>
-      <c r="G183" s="12"/>
-      <c r="H183" s="12"/>
-      <c r="I183" s="12"/>
-      <c r="J183" s="12"/>
-      <c r="K183" s="12"/>
-      <c r="L183" s="12"/>
-      <c r="M183" s="12"/>
-      <c r="N183" s="13"/>
-    </row>
-    <row r="184" spans="5:14">
-      <c r="E184" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="F184" s="12"/>
-      <c r="G184" s="12"/>
-      <c r="H184" s="12"/>
-      <c r="I184" s="12"/>
-      <c r="J184" s="12"/>
-      <c r="K184" s="12"/>
-      <c r="L184" s="12"/>
-      <c r="M184" s="12"/>
-      <c r="N184" s="13"/>
-    </row>
-    <row r="185" spans="5:14">
-      <c r="E185" s="11"/>
-      <c r="F185" s="12"/>
-      <c r="G185" s="12"/>
-      <c r="H185" s="12"/>
-      <c r="I185" s="12"/>
-      <c r="J185" s="12"/>
-      <c r="K185" s="12"/>
-      <c r="L185" s="12"/>
-      <c r="M185" s="12"/>
-      <c r="N185" s="13"/>
-    </row>
-    <row r="186" spans="5:14">
-      <c r="E186" s="11"/>
-      <c r="F186" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="G186" s="12"/>
-      <c r="H186" s="12"/>
-      <c r="I186" s="12"/>
-      <c r="J186" s="12"/>
-      <c r="K186" s="12"/>
-      <c r="L186" s="12"/>
-      <c r="M186" s="12"/>
-      <c r="N186" s="13"/>
-    </row>
-    <row r="187" spans="5:14">
-      <c r="E187" s="11"/>
-      <c r="F187" s="12"/>
-      <c r="G187" s="12"/>
-      <c r="H187" s="12"/>
-      <c r="I187" s="12"/>
-      <c r="J187" s="12"/>
-      <c r="K187" s="12"/>
-      <c r="L187" s="12"/>
-      <c r="M187" s="12"/>
-      <c r="N187" s="13"/>
-    </row>
-    <row r="188" spans="5:14">
-      <c r="E188" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F188" s="12"/>
-      <c r="G188" s="12"/>
-      <c r="H188" s="12"/>
-      <c r="I188" s="12"/>
-      <c r="J188" s="12"/>
-      <c r="K188" s="12"/>
-      <c r="L188" s="12"/>
-      <c r="M188" s="12"/>
-      <c r="N188" s="13"/>
-    </row>
-    <row r="189" spans="5:14">
-      <c r="E189" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F189" s="12"/>
-      <c r="G189" s="12"/>
-      <c r="H189" s="12"/>
-      <c r="I189" s="12"/>
-      <c r="J189" s="12"/>
-      <c r="K189" s="12"/>
-      <c r="L189" s="12"/>
-      <c r="M189" s="12"/>
-      <c r="N189" s="13"/>
-    </row>
-    <row r="190" spans="5:14">
-      <c r="E190" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="F190" s="19"/>
-      <c r="G190" s="19"/>
-      <c r="H190" s="19"/>
-      <c r="I190" s="19"/>
-      <c r="J190" s="19"/>
-      <c r="K190" s="19"/>
-      <c r="L190" s="19"/>
-      <c r="M190" s="12"/>
-      <c r="N190" s="13"/>
-    </row>
-    <row r="191" spans="5:14">
-      <c r="E191" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="F191" s="19"/>
-      <c r="G191" s="19"/>
-      <c r="H191" s="19"/>
-      <c r="I191" s="19"/>
-      <c r="J191" s="19"/>
-      <c r="K191" s="19"/>
-      <c r="L191" s="19"/>
-      <c r="M191" s="12"/>
-      <c r="N191" s="13"/>
-    </row>
-    <row r="192" spans="5:14">
-      <c r="E192" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F192" s="19"/>
-      <c r="G192" s="19"/>
-      <c r="H192" s="19"/>
-      <c r="I192" s="19"/>
-      <c r="J192" s="19"/>
-      <c r="K192" s="19"/>
-      <c r="L192" s="19"/>
-      <c r="M192" s="12"/>
-      <c r="N192" s="13"/>
-    </row>
-    <row r="193" spans="5:14">
-      <c r="E193" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F193" s="19"/>
-      <c r="G193" s="19"/>
-      <c r="H193" s="19"/>
-      <c r="I193" s="19"/>
-      <c r="J193" s="19"/>
-      <c r="K193" s="19"/>
-      <c r="L193" s="19"/>
-      <c r="M193" s="12"/>
-      <c r="N193" s="13"/>
-    </row>
-    <row r="194" spans="5:14">
-      <c r="E194" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="F194" s="19"/>
-      <c r="G194" s="19"/>
-      <c r="H194" s="19"/>
-      <c r="I194" s="19"/>
-      <c r="J194" s="19"/>
-      <c r="K194" s="19"/>
-      <c r="L194" s="19"/>
-      <c r="M194" s="12"/>
-      <c r="N194" s="13"/>
-    </row>
-    <row r="195" spans="5:14">
-      <c r="E195" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F195" s="19"/>
-      <c r="G195" s="19"/>
-      <c r="H195" s="19"/>
-      <c r="I195" s="19"/>
-      <c r="J195" s="19"/>
-      <c r="K195" s="19"/>
-      <c r="L195" s="19"/>
-      <c r="M195" s="12"/>
-      <c r="N195" s="13"/>
-    </row>
-    <row r="196" spans="5:14">
-      <c r="E196" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="F196" s="21"/>
-      <c r="G196" s="21"/>
-      <c r="H196" s="21"/>
-      <c r="I196" s="21"/>
-      <c r="J196" s="21"/>
-      <c r="K196" s="21"/>
-      <c r="L196" s="21"/>
-      <c r="M196" s="15"/>
-      <c r="N196" s="16"/>
-    </row>
-    <row r="198" spans="5:14">
-      <c r="E198" s="5" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="199" spans="5:14">
-      <c r="E199" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="200" spans="5:14">
-      <c r="E200" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="202" spans="5:14">
-      <c r="E202" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="203" spans="5:14">
-      <c r="E203" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="204" spans="5:14">
-      <c r="E204" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="205" spans="5:14">
-      <c r="E205" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="207" spans="5:14">
-      <c r="E207" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="208" spans="5:14">
-      <c r="E208" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="210" spans="3:5">
-      <c r="C210" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="D210" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="212" spans="3:5">
-      <c r="D212" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E212" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="213" spans="3:5">
-      <c r="E213" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="214" spans="3:5">
-      <c r="D214" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E214" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="215" spans="3:5">
-      <c r="D215" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E215" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="216" spans="3:5">
-      <c r="E216" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="218" spans="3:5">
-      <c r="D218" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E218" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="219" spans="3:5">
-      <c r="E219" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="220" spans="3:5">
-      <c r="E220" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="221" spans="3:5">
-      <c r="E221" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="222" spans="3:5">
-      <c r="E222" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="223" spans="3:5">
-      <c r="E223" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="224" spans="3:5">
-      <c r="E224" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="227" spans="4:4">
-      <c r="D227" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="228" spans="4:4">
-      <c r="D228" s="23"/>
-    </row>
-    <row r="255" spans="2:4">
-      <c r="B255" s="22">
-        <v>3</v>
-      </c>
-      <c r="C255" s="25" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="256" spans="2:4">
-      <c r="C256" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="D256" s="5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="257" spans="4:5">
-      <c r="D257" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="E257" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="258" spans="4:5">
-      <c r="D258" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E258" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="259" spans="4:5">
-      <c r="D259" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E259" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="260" spans="4:5">
-      <c r="E260" s="5" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="261" spans="4:5">
-      <c r="E261" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="262" spans="4:5">
-      <c r="E262" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="263" spans="4:5">
-      <c r="E263" s="5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="264" spans="4:5">
-      <c r="E264" s="5" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="265" spans="4:5">
-      <c r="E265" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="266" spans="4:5">
-      <c r="E266" s="5" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="267" spans="4:5">
-      <c r="E267" s="5" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="268" spans="4:5">
-      <c r="E268" s="5" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="269" spans="4:5">
-      <c r="E269" s="5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="273" spans="3:5">
-      <c r="D273" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="E273" s="5" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="274" spans="3:5">
-      <c r="E274" s="5" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="275" spans="3:5">
-      <c r="E275" s="5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="277" spans="3:5">
-      <c r="C277" s="24" t="s">
-        <v>283</v>
-      </c>
-      <c r="D277" s="5" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="278" spans="3:5">
-      <c r="D278" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="E278" s="5" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="279" spans="3:5">
-      <c r="D279" s="5">
-        <v>1</v>
-      </c>
-      <c r="E279" s="6" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="280" spans="3:5">
-      <c r="E280" s="5" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="281" spans="3:5">
-      <c r="E281" s="5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="282" spans="3:5">
-      <c r="E282" s="5" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="283" spans="3:5">
-      <c r="E283" s="6" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="285" spans="3:5">
-      <c r="D285" s="5">
-        <v>2</v>
-      </c>
-      <c r="E285" s="5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="286" spans="3:5">
-      <c r="E286" s="6" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="287" spans="3:5">
-      <c r="E287" s="5" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="288" spans="3:5">
-      <c r="E288" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="289" spans="2:5">
-      <c r="E289" s="5" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="295" spans="2:5">
-      <c r="B295" s="22">
-        <v>4</v>
-      </c>
-      <c r="C295" s="24" t="s">
-        <v>276</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A1" location="目录!A1" tooltip="返回目录" display="返回"/>
-    <hyperlink ref="B12" location="Git_与远程主机的交互" tooltip="Git_与远程主机的交互" display="与远程仓库交互"/>
-    <hyperlink ref="B6" location="Git_管理本地仓库" tooltip="Git_管理本地仓库" display="管理本地仓库"/>
-    <hyperlink ref="B13" location="Git_配置" tooltip="Git_配置" display="git配置"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4437,11 +4720,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0"/>
   <cols>
@@ -4493,13 +4774,13 @@
     <row r="8" spans="1:4">
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="C9" s="5"/>
       <c r="D9" s="2" t="s">
-        <v>277</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4526,27 +4807,32 @@
     </row>
     <row r="14" spans="1:4">
       <c r="D14" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="D15" s="2" t="s">
-        <v>278</v>
+        <v>328</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="D16" s="1" t="s">
-        <v>275</v>
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="4:4">
       <c r="D32" s="1" t="s">
-        <v>280</v>
+        <v>331</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="1" t="s">
-        <v>281</v>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
How to find real JDK directory in Mac
</commit_message>
<xml_diff>
--- a/NoteBook.xlsx
+++ b/NoteBook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8560" yWindow="2240" windowWidth="25520" windowHeight="15540" tabRatio="760" activeTab="8"/>
+    <workbookView xWindow="12860" yWindow="1580" windowWidth="25520" windowHeight="15540" tabRatio="760" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="目录" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="1575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="1646">
   <si>
     <t>#else</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -6613,10 +6613,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Java </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Xcocde配置 Architectures</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -7140,6 +7136,237 @@
   </si>
   <si>
     <t>删除 find ./ -type f -name '.svn' -exec rm -rf {} \;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>总结</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ which java</t>
+  </si>
+  <si>
+    <t>$ ls -l /usr/bin/java</t>
+  </si>
+  <si>
+    <t>$ ls /System/Library/Frameworks/JavaVM.framework/Versions/Current/Commands</t>
+  </si>
+  <si>
+    <t>appletviewer</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>javapackager</t>
+  </si>
+  <si>
+    <t>jdeps</t>
+  </si>
+  <si>
+    <t>jmap</t>
+  </si>
+  <si>
+    <t>jstack</t>
+  </si>
+  <si>
+    <t>orbd</t>
+  </si>
+  <si>
+    <t>schemagen</t>
+  </si>
+  <si>
+    <t>wsimport</t>
+  </si>
+  <si>
+    <t>apt</t>
+  </si>
+  <si>
+    <t>java_home</t>
+  </si>
+  <si>
+    <t>javaws</t>
+  </si>
+  <si>
+    <t>jhat</t>
+  </si>
+  <si>
+    <t>jmc</t>
+  </si>
+  <si>
+    <t>jstat</t>
+  </si>
+  <si>
+    <t>pack200</t>
+  </si>
+  <si>
+    <t>serialver</t>
+  </si>
+  <si>
+    <t>xjc</t>
+  </si>
+  <si>
+    <t>extcheck</t>
+  </si>
+  <si>
+    <t>javac</t>
+  </si>
+  <si>
+    <t>jcmd</t>
+  </si>
+  <si>
+    <t>jhsdb</t>
+  </si>
+  <si>
+    <t>jps</t>
+  </si>
+  <si>
+    <t>jstatd</t>
+  </si>
+  <si>
+    <t>policytool</t>
+  </si>
+  <si>
+    <t>servertool</t>
+  </si>
+  <si>
+    <t>idlj</t>
+  </si>
+  <si>
+    <t>javadoc</t>
+  </si>
+  <si>
+    <t>jconsole</t>
+  </si>
+  <si>
+    <t>jimage</t>
+  </si>
+  <si>
+    <t>jrunscript</t>
+  </si>
+  <si>
+    <t>jvisualvm</t>
+  </si>
+  <si>
+    <t>rmic</t>
+  </si>
+  <si>
+    <t>tnameserv</t>
+  </si>
+  <si>
+    <t>jar</t>
+  </si>
+  <si>
+    <t>javah</t>
+  </si>
+  <si>
+    <t>jcontrol</t>
+  </si>
+  <si>
+    <t>jinfo</t>
+  </si>
+  <si>
+    <t>jsadebugd</t>
+  </si>
+  <si>
+    <t>keytool</t>
+  </si>
+  <si>
+    <t>rmid</t>
+  </si>
+  <si>
+    <t>unpack200</t>
+  </si>
+  <si>
+    <t>jarsigner</t>
+  </si>
+  <si>
+    <t>javap</t>
+  </si>
+  <si>
+    <t>jdb</t>
+  </si>
+  <si>
+    <t>jjs</t>
+  </si>
+  <si>
+    <t>jshell</t>
+  </si>
+  <si>
+    <t>native2ascii</t>
+  </si>
+  <si>
+    <t>rmiregistry</t>
+  </si>
+  <si>
+    <t>wsgen</t>
+  </si>
+  <si>
+    <t>$ ls -l /Library/Java/JavaVirtualMachines/jdk1.7.0_79.jdk/Contents/Home</t>
+  </si>
+  <si>
+    <t>total 39824</t>
+  </si>
+  <si>
+    <t>-rw-rw-r--   1 Sam  wheel      3339  4 11  2015 COPYRIGHT</t>
+  </si>
+  <si>
+    <t>-rw-rw-r--   1 Sam  wheel        40  4 11  2015 LICENSE</t>
+  </si>
+  <si>
+    <t>-rw-rw-r--   1 Sam  wheel       114  4 11  2015 README.html</t>
+  </si>
+  <si>
+    <t>-rw-rw-r--   1 Sam  wheel    110114  3 17  2015 THIRDPARTYLICENSEREADME-JAVAFX.txt</t>
+  </si>
+  <si>
+    <t>-rw-rw-r--   1 Sam  wheel    173571  4 11  2015 THIRDPARTYLICENSEREADME.txt</t>
+  </si>
+  <si>
+    <t>drwxrwxr-x  44 Sam  wheel      1496  4 11  2015 bin</t>
+  </si>
+  <si>
+    <t>drwxrwxr-x   9 Sam  wheel       306  4 11  2015 db</t>
+  </si>
+  <si>
+    <t>drwxrwxr-x   9 Sam  wheel       306  4 11  2015 include</t>
+  </si>
+  <si>
+    <t>drwxrwxr-x  10 Sam  wheel       340  4 11  2015 jre</t>
+  </si>
+  <si>
+    <t>drwxrwxr-x  14 Sam  wheel       476  4 11  2015 lib</t>
+  </si>
+  <si>
+    <t>drwxrwxr-x   5 Sam  wheel       170  4 11  2015 man</t>
+  </si>
+  <si>
+    <t>-rw-rw-r--   1 Sam  wheel       502  4 11  2015 release</t>
+  </si>
+  <si>
+    <t>-rw-rw-r--   1 Sam  wheel  20084963  4 11  2015 src.zip</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">lrwxr-xr-x  1 Sam  wheel  74 10  9  2016 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体 (正文)"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/usr/bin/java -&gt; /System/Library/Frameworks/JavaVM.framework/Versions/Current/Commands/java</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ cd /System/Library/Frameworks/JavaVM.framework/Versions/Current/Commands</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ ./java_home</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -10656,7 +10883,7 @@
     </row>
     <row r="6" spans="2:3">
       <c r="C6" s="2" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="9" spans="2:3">
@@ -10756,7 +10983,7 @@
         <v>3</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -10764,7 +10991,7 @@
         <v>4</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -10772,7 +10999,7 @@
         <v>5</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -10780,7 +11007,7 @@
         <v>6</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -10921,7 +11148,7 @@
       <c r="C58" s="6"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="59" spans="2:5" s="8" customFormat="1">
@@ -11065,7 +11292,7 @@
     </row>
     <row r="88" spans="2:4">
       <c r="D88" s="2" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="92" spans="2:4">
@@ -11073,12 +11300,12 @@
         <v>7</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="93" spans="2:4">
       <c r="D93" s="2" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="97" spans="2:4">
@@ -16412,11 +16639,9 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E143"/>
+  <dimension ref="A1:Q173"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="B144" sqref="B144"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
   <cols>
@@ -16677,29 +16902,306 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="134" spans="2:4">
+    <row r="134" spans="3:4">
       <c r="D134" s="37" t="s">
         <v>1267</v>
       </c>
     </row>
-    <row r="135" spans="2:4">
+    <row r="135" spans="3:4">
       <c r="D135" s="73" t="s">
         <v>1192</v>
       </c>
     </row>
-    <row r="136" spans="2:4">
+    <row r="136" spans="3:4">
       <c r="D136" s="37" t="s">
         <v>1193</v>
       </c>
     </row>
-    <row r="137" spans="2:4">
+    <row r="137" spans="3:4">
       <c r="D137" s="37" t="s">
         <v>1194</v>
       </c>
     </row>
-    <row r="143" spans="2:4">
-      <c r="B143" s="37" t="s">
-        <v>1466</v>
+    <row r="143" spans="3:4">
+      <c r="C143" s="37" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="145" spans="3:17">
+      <c r="C145" s="37" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="146" spans="3:17">
+      <c r="C146" s="37" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="147" spans="3:17">
+      <c r="C147" s="37" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="148" spans="3:17">
+      <c r="C148" s="37" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="149" spans="3:17">
+      <c r="C149" s="37" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="150" spans="3:17">
+      <c r="C150" s="37" t="s">
+        <v>1578</v>
+      </c>
+      <c r="D150" s="37" t="s">
+        <v>1579</v>
+      </c>
+      <c r="F150" s="37" t="s">
+        <v>1580</v>
+      </c>
+      <c r="G150" s="37" t="s">
+        <v>1581</v>
+      </c>
+      <c r="I150" s="37" t="s">
+        <v>1582</v>
+      </c>
+      <c r="K150" s="37" t="s">
+        <v>1583</v>
+      </c>
+      <c r="M150" s="37" t="s">
+        <v>1584</v>
+      </c>
+      <c r="O150" s="37" t="s">
+        <v>1585</v>
+      </c>
+      <c r="P150" s="37" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="151" spans="3:17">
+      <c r="C151" s="37" t="s">
+        <v>1587</v>
+      </c>
+      <c r="E151" s="37" t="s">
+        <v>1588</v>
+      </c>
+      <c r="F151" s="37" t="s">
+        <v>1589</v>
+      </c>
+      <c r="H151" s="37" t="s">
+        <v>1590</v>
+      </c>
+      <c r="J151" s="37" t="s">
+        <v>1591</v>
+      </c>
+      <c r="L151" s="37" t="s">
+        <v>1592</v>
+      </c>
+      <c r="N151" s="37" t="s">
+        <v>1593</v>
+      </c>
+      <c r="P151" s="37" t="s">
+        <v>1594</v>
+      </c>
+      <c r="Q151" s="37" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="152" spans="3:17">
+      <c r="C152" s="37" t="s">
+        <v>1596</v>
+      </c>
+      <c r="D152" s="37" t="s">
+        <v>1597</v>
+      </c>
+      <c r="F152" s="37" t="s">
+        <v>1598</v>
+      </c>
+      <c r="H152" s="37" t="s">
+        <v>1599</v>
+      </c>
+      <c r="J152" s="37" t="s">
+        <v>1600</v>
+      </c>
+      <c r="L152" s="37" t="s">
+        <v>1601</v>
+      </c>
+      <c r="N152" s="37" t="s">
+        <v>1602</v>
+      </c>
+      <c r="O152" s="37" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="153" spans="3:17">
+      <c r="C153" s="37" t="s">
+        <v>1604</v>
+      </c>
+      <c r="E153" s="37" t="s">
+        <v>1605</v>
+      </c>
+      <c r="G153" s="37" t="s">
+        <v>1606</v>
+      </c>
+      <c r="H153" s="37" t="s">
+        <v>1607</v>
+      </c>
+      <c r="J153" s="37" t="s">
+        <v>1608</v>
+      </c>
+      <c r="K153" s="37" t="s">
+        <v>1609</v>
+      </c>
+      <c r="L153" s="37" t="s">
+        <v>1610</v>
+      </c>
+      <c r="N153" s="37" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="154" spans="3:17">
+      <c r="C154" s="37" t="s">
+        <v>1612</v>
+      </c>
+      <c r="E154" s="37" t="s">
+        <v>1613</v>
+      </c>
+      <c r="G154" s="37" t="s">
+        <v>1614</v>
+      </c>
+      <c r="H154" s="37" t="s">
+        <v>1615</v>
+      </c>
+      <c r="J154" s="37" t="s">
+        <v>1616</v>
+      </c>
+      <c r="K154" s="37" t="s">
+        <v>1617</v>
+      </c>
+      <c r="M154" s="37" t="s">
+        <v>1618</v>
+      </c>
+      <c r="O154" s="37" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="155" spans="3:17">
+      <c r="C155" s="37" t="s">
+        <v>1620</v>
+      </c>
+      <c r="D155" s="37" t="s">
+        <v>1621</v>
+      </c>
+      <c r="F155" s="37" t="s">
+        <v>1622</v>
+      </c>
+      <c r="H155" s="37" t="s">
+        <v>1623</v>
+      </c>
+      <c r="J155" s="37" t="s">
+        <v>1624</v>
+      </c>
+      <c r="L155" s="37" t="s">
+        <v>1625</v>
+      </c>
+      <c r="M155" s="37" t="s">
+        <v>1626</v>
+      </c>
+      <c r="N155" s="37" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="156" spans="3:17">
+      <c r="C156" s="44" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="157" spans="3:17">
+      <c r="C157" s="44" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="158" spans="3:17">
+      <c r="C158" s="44" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="159" spans="3:17">
+      <c r="C159" s="37" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="160" spans="3:17">
+      <c r="C160" s="37" t="s">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="161" spans="3:3">
+      <c r="C161" s="37" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="162" spans="3:3">
+      <c r="C162" s="37" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="163" spans="3:3">
+      <c r="C163" s="37" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="164" spans="3:3">
+      <c r="C164" s="37" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="165" spans="3:3">
+      <c r="C165" s="37" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="166" spans="3:3">
+      <c r="C166" s="37" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="167" spans="3:3">
+      <c r="C167" s="37" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="168" spans="3:3">
+      <c r="C168" s="37" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="169" spans="3:3">
+      <c r="C169" s="37" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="170" spans="3:3">
+      <c r="C170" s="37" t="s">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="171" spans="3:3">
+      <c r="C171" s="37" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="172" spans="3:3">
+      <c r="C172" s="37" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="173" spans="3:3">
+      <c r="C173" s="37" t="s">
+        <v>1642</v>
       </c>
     </row>
   </sheetData>
@@ -17954,17 +18456,17 @@
         <v>2</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="C8" s="37" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="C10" s="37" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -17972,12 +18474,12 @@
         <v>3</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="C13" s="37" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="20" spans="2:3">
@@ -21189,27 +21691,27 @@
     </row>
     <row r="62" spans="2:6">
       <c r="B62" s="2" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="64" spans="2:6">
       <c r="B64" s="2" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="2" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="2" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" s="2" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
   </sheetData>
@@ -21953,65 +22455,65 @@
         <v>4</v>
       </c>
       <c r="C111" s="106" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="112" spans="2:4">
       <c r="C112" s="3" t="s">
+        <v>1496</v>
+      </c>
+      <c r="D112" s="3" t="s">
         <v>1497</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>1498</v>
       </c>
     </row>
     <row r="113" spans="3:4">
       <c r="D113" s="3" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="114" spans="3:4">
       <c r="D114" s="3" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="116" spans="3:4">
       <c r="C116" s="3" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="117" spans="3:4">
       <c r="D117" s="3" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="127" spans="3:4">
       <c r="D127" s="3" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="140" spans="4:4">
       <c r="D140" s="3" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="141" spans="4:4">
       <c r="D141" s="3" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="142" spans="4:4">
       <c r="D142" s="3" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="160" spans="4:4">
       <c r="D160" s="3" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="161" spans="4:4">
       <c r="D161" s="3" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="177" spans="2:4">
@@ -22019,140 +22521,140 @@
         <v>5</v>
       </c>
       <c r="C177" s="106" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="179" spans="2:4">
       <c r="C179" s="3" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D179" s="3" t="s">
         <v>1522</v>
-      </c>
-      <c r="D179" s="3" t="s">
-        <v>1523</v>
       </c>
     </row>
     <row r="180" spans="2:4">
       <c r="D180" s="3" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="181" spans="2:4">
       <c r="D181" s="3" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="182" spans="2:4">
       <c r="D182" s="3" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="183" spans="2:4">
       <c r="D183" s="3" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="185" spans="2:4">
       <c r="C185" s="3" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="186" spans="2:4">
       <c r="D186" s="3" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="194" spans="4:4">
       <c r="D194" s="3" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="195" spans="4:4">
       <c r="D195" s="3" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="197" spans="4:4">
       <c r="D197" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="198" spans="4:4">
       <c r="D198" s="3" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="199" spans="4:4">
       <c r="D199" s="3" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="200" spans="4:4">
       <c r="D200" s="3" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="201" spans="4:4">
       <c r="D201" s="3" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="202" spans="4:4">
       <c r="D202" s="3" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="204" spans="4:4">
       <c r="D204" s="3" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="205" spans="4:4">
       <c r="D205" s="3" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="206" spans="4:4">
       <c r="D206" s="3" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="208" spans="4:4">
       <c r="D208" s="3" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="209" spans="4:4">
       <c r="D209" s="3" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="223" spans="4:4">
       <c r="D223" s="3" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="224" spans="4:4">
       <c r="D224" s="3" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="227" spans="4:4">
       <c r="D227" s="3" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="228" spans="4:4">
       <c r="D228" s="3" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="230" spans="4:4">
       <c r="D230" s="3" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="231" spans="4:4">
       <c r="D231" s="3" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="303" spans="2:3">
@@ -22160,7 +22662,7 @@
         <v>5</v>
       </c>
       <c r="C303" s="3" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="305" spans="2:13">
@@ -22168,56 +22670,56 @@
         <v>6</v>
       </c>
       <c r="C305" s="3" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="306" spans="2:13">
       <c r="C306" s="3" t="s">
+        <v>1552</v>
+      </c>
+      <c r="D306" s="3" t="s">
         <v>1553</v>
-      </c>
-      <c r="D306" s="3" t="s">
-        <v>1554</v>
       </c>
     </row>
     <row r="307" spans="2:13">
       <c r="D307" s="3" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="308" spans="2:13">
       <c r="D308" s="3" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="309" spans="2:13">
       <c r="C309" s="3" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="310" spans="2:13">
       <c r="C310" s="3" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="312" spans="2:13">
       <c r="C312" s="3" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="H312" s="3" t="s">
+        <v>1558</v>
+      </c>
+      <c r="M312" s="3" t="s">
         <v>1559</v>
-      </c>
-      <c r="M312" s="3" t="s">
-        <v>1560</v>
       </c>
     </row>
     <row r="320" spans="2:13">
       <c r="C320" s="3" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="321" spans="3:3">
       <c r="C321" s="3" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="324" spans="3:3">
@@ -22876,7 +23378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q128"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
   <cols>
@@ -23297,40 +23799,40 @@
         <v>103</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="90" spans="2:17">
       <c r="D90" s="2" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="91" spans="2:17">
       <c r="C91" s="2" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="93" spans="2:17">
       <c r="D93" s="2" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="95" spans="2:17">
       <c r="D95" s="2" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="96" spans="2:17">
       <c r="D96" s="2" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="97" spans="4:17">
       <c r="D97" s="90" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="E97" s="91"/>
       <c r="F97" s="91"/>
@@ -23348,7 +23850,7 @@
     </row>
     <row r="98" spans="4:17">
       <c r="D98" s="96" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="E98" s="94"/>
       <c r="F98" s="94"/>
@@ -23366,7 +23868,7 @@
     </row>
     <row r="99" spans="4:17">
       <c r="D99" s="96" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="E99" s="94"/>
       <c r="F99" s="94"/>
@@ -23384,10 +23886,10 @@
     </row>
     <row r="100" spans="4:17">
       <c r="D100" s="96" t="s">
+        <v>1475</v>
+      </c>
+      <c r="E100" s="94" t="s">
         <v>1476</v>
-      </c>
-      <c r="E100" s="94" t="s">
-        <v>1477</v>
       </c>
       <c r="F100" s="94"/>
       <c r="G100" s="94"/>
@@ -23404,7 +23906,7 @@
     </row>
     <row r="101" spans="4:17">
       <c r="D101" s="96" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="E101" s="94"/>
       <c r="F101" s="94"/>
@@ -23422,10 +23924,10 @@
     </row>
     <row r="102" spans="4:17">
       <c r="D102" s="96" t="s">
+        <v>1477</v>
+      </c>
+      <c r="E102" s="94" t="s">
         <v>1478</v>
-      </c>
-      <c r="E102" s="94" t="s">
-        <v>1479</v>
       </c>
       <c r="F102" s="94"/>
       <c r="G102" s="94"/>
@@ -23442,7 +23944,7 @@
     </row>
     <row r="103" spans="4:17">
       <c r="D103" s="96" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="E103" s="94"/>
       <c r="F103" s="94"/>
@@ -23460,10 +23962,10 @@
     </row>
     <row r="104" spans="4:17">
       <c r="D104" s="96" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="E104" s="94" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="F104" s="94"/>
       <c r="G104" s="94"/>
@@ -23480,7 +23982,7 @@
     </row>
     <row r="105" spans="4:17">
       <c r="D105" s="96" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="E105" s="94"/>
       <c r="F105" s="94"/>
@@ -23498,10 +24000,10 @@
     </row>
     <row r="106" spans="4:17">
       <c r="D106" s="96" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="E106" s="94" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="F106" s="94"/>
       <c r="G106" s="94"/>
@@ -23518,7 +24020,7 @@
     </row>
     <row r="107" spans="4:17">
       <c r="D107" s="96" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="E107" s="94"/>
       <c r="F107" s="94"/>
@@ -23536,10 +24038,10 @@
     </row>
     <row r="108" spans="4:17">
       <c r="D108" s="96" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="E108" s="94" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="F108" s="94"/>
       <c r="G108" s="94"/>
@@ -23556,10 +24058,10 @@
     </row>
     <row r="109" spans="4:17">
       <c r="D109" s="96" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="E109" s="94" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="F109" s="94"/>
       <c r="G109" s="94"/>
@@ -23576,10 +24078,10 @@
     </row>
     <row r="110" spans="4:17">
       <c r="D110" s="96" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="E110" s="94" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="F110" s="94"/>
       <c r="G110" s="94"/>
@@ -23596,10 +24098,10 @@
     </row>
     <row r="111" spans="4:17">
       <c r="D111" s="96" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="E111" s="94" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="F111" s="94"/>
       <c r="G111" s="94"/>
@@ -23638,7 +24140,7 @@
         <v>103</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="117" spans="2:4">
@@ -23646,32 +24148,32 @@
         <v>145</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="118" spans="2:4">
       <c r="D118" s="5" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="120" spans="2:4">
       <c r="D120" s="2" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="121" spans="2:4">
       <c r="D121" s="5" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="122" spans="2:4">
       <c r="D122" s="5" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="123" spans="2:4">
       <c r="D123" s="2" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="125" spans="2:4">
@@ -23682,20 +24184,20 @@
         <v>103</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="127" spans="2:4">
       <c r="C127" s="2" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="128" spans="2:4">
       <c r="D128" s="5" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>